<commit_message>
Finish update_qcsda function for both Google Drive and local disk and add missing credits (NumPy) to README.md file
</commit_message>
<xml_diff>
--- a/qcdata/QCSDA.xlsx
+++ b/qcdata/QCSDA.xlsx
@@ -14,6 +14,9 @@
     <sheet name="Redo_distortion_10-08-2021" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Redo_force_10-08-2021" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Redo_COG_10-08-2021" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Redo_distortion_2021-08-10" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Redo_force_2021-08-10" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Redo_COG_2021-08-10" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1506,6 +1509,1890 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B1" t="n">
+        <v>5001</v>
+      </c>
+      <c r="C1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" t="n">
+        <v>68.77999877929688</v>
+      </c>
+      <c r="F1" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G1" t="n">
+        <v>3500000</v>
+      </c>
+      <c r="H1" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5001</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="n">
+        <v>68.79000091552734</v>
+      </c>
+      <c r="F2" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3500000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5301</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>68.26999664306641</v>
+      </c>
+      <c r="F3" t="n">
+        <v>505000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3503000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5002</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>69.37000274658203</v>
+      </c>
+      <c r="F4" t="n">
+        <v>500030</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3500030</v>
+      </c>
+      <c r="H4" t="n">
+        <v>150.2100067138672</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5302</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" t="n">
+        <v>69.51000213623047</v>
+      </c>
+      <c r="F5" t="n">
+        <v>505030</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3503030</v>
+      </c>
+      <c r="H5" t="n">
+        <v>160.2100067138672</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5003</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>68.05999755859375</v>
+      </c>
+      <c r="F6" t="n">
+        <v>500060</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3500060</v>
+      </c>
+      <c r="H6" t="n">
+        <v>150.4199981689453</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5004</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>69.41000366210938</v>
+      </c>
+      <c r="F7" t="n">
+        <v>500090</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3500090</v>
+      </c>
+      <c r="H7" t="n">
+        <v>150.6300048828125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B8" t="n">
+        <v>5304</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>69.16000366210938</v>
+      </c>
+      <c r="F8" t="n">
+        <v>505090</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3503090</v>
+      </c>
+      <c r="H8" t="n">
+        <v>160.6300048828125</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B9" t="n">
+        <v>5306</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" t="n">
+        <v>69.58000183105469</v>
+      </c>
+      <c r="F9" t="n">
+        <v>505150</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3503150</v>
+      </c>
+      <c r="H9" t="n">
+        <v>161.0500030517578</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B10" t="n">
+        <v>5307</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" t="n">
+        <v>69.95999908447266</v>
+      </c>
+      <c r="F10" t="n">
+        <v>505180</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3503180</v>
+      </c>
+      <c r="H10" t="n">
+        <v>161.2599945068359</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B11" t="n">
+        <v>5008</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>69.22000122070312</v>
+      </c>
+      <c r="F11" t="n">
+        <v>500210</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3500210</v>
+      </c>
+      <c r="H11" t="n">
+        <v>151.4700012207031</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B12" t="n">
+        <v>5308</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>7</v>
+      </c>
+      <c r="E12" t="n">
+        <v>69.66999816894531</v>
+      </c>
+      <c r="F12" t="n">
+        <v>505210</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3503210</v>
+      </c>
+      <c r="H12" t="n">
+        <v>161.4700012207031</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B13" t="n">
+        <v>5009</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="n">
+        <v>69.04000091552734</v>
+      </c>
+      <c r="F13" t="n">
+        <v>500240</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3500240</v>
+      </c>
+      <c r="H13" t="n">
+        <v>151.6799926757812</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B14" t="n">
+        <v>5309</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E14" t="n">
+        <v>68.05000305175781</v>
+      </c>
+      <c r="F14" t="n">
+        <v>505240</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3503240</v>
+      </c>
+      <c r="H14" t="n">
+        <v>161.6799926757812</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B15" t="n">
+        <v>5309</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>8</v>
+      </c>
+      <c r="E15" t="n">
+        <v>68.01999664306641</v>
+      </c>
+      <c r="F15" t="n">
+        <v>505240</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3503240</v>
+      </c>
+      <c r="H15" t="n">
+        <v>161.6799926757812</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B16" t="n">
+        <v>5010</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" t="n">
+        <v>69.98999786376953</v>
+      </c>
+      <c r="F16" t="n">
+        <v>500270</v>
+      </c>
+      <c r="G16" t="n">
+        <v>3500270</v>
+      </c>
+      <c r="H16" t="n">
+        <v>151.8899993896484</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B17" t="n">
+        <v>5310</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" t="n">
+        <v>69.94000244140625</v>
+      </c>
+      <c r="F17" t="n">
+        <v>505270</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3503270</v>
+      </c>
+      <c r="H17" t="n">
+        <v>161.8899993896484</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B18" t="n">
+        <v>5311</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="n">
+        <v>6</v>
+      </c>
+      <c r="E18" t="n">
+        <v>68.95999908447266</v>
+      </c>
+      <c r="F18" t="n">
+        <v>505300</v>
+      </c>
+      <c r="G18" t="n">
+        <v>3503300</v>
+      </c>
+      <c r="H18" t="n">
+        <v>162.1000061035156</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B19" t="n">
+        <v>5012</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>68.37000274658203</v>
+      </c>
+      <c r="F19" t="n">
+        <v>500330</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3500330</v>
+      </c>
+      <c r="H19" t="n">
+        <v>152.3099975585938</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B20" t="n">
+        <v>5312</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" t="n">
+        <v>6</v>
+      </c>
+      <c r="E20" t="n">
+        <v>68.09999847412109</v>
+      </c>
+      <c r="F20" t="n">
+        <v>505330</v>
+      </c>
+      <c r="G20" t="n">
+        <v>3503330</v>
+      </c>
+      <c r="H20" t="n">
+        <v>162.3099975585938</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B21" t="n">
+        <v>5015</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" t="n">
+        <v>68.45999908447266</v>
+      </c>
+      <c r="F21" t="n">
+        <v>500420</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3500420</v>
+      </c>
+      <c r="H21" t="n">
+        <v>152.9400024414062</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B22" t="n">
+        <v>5016</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>4</v>
+      </c>
+      <c r="E22" t="n">
+        <v>68.68000030517578</v>
+      </c>
+      <c r="F22" t="n">
+        <v>500450</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3500450</v>
+      </c>
+      <c r="H22" t="n">
+        <v>153.1499938964844</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B23" t="n">
+        <v>5018</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>68.01999664306641</v>
+      </c>
+      <c r="F23" t="n">
+        <v>500510</v>
+      </c>
+      <c r="G23" t="n">
+        <v>3500510</v>
+      </c>
+      <c r="H23" t="n">
+        <v>153.5700073242188</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B24" t="n">
+        <v>5319</v>
+      </c>
+      <c r="C24" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" t="n">
+        <v>6</v>
+      </c>
+      <c r="E24" t="n">
+        <v>69.73000335693359</v>
+      </c>
+      <c r="F24" t="n">
+        <v>505540</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3503540</v>
+      </c>
+      <c r="H24" t="n">
+        <v>163.7799987792969</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B25" t="n">
+        <v>5020</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>69.29000091552734</v>
+      </c>
+      <c r="F25" t="n">
+        <v>500570</v>
+      </c>
+      <c r="G25" t="n">
+        <v>3500570</v>
+      </c>
+      <c r="H25" t="n">
+        <v>153.9900054931641</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B26" t="n">
+        <v>5320</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" t="n">
+        <v>8</v>
+      </c>
+      <c r="E26" t="n">
+        <v>68.13999938964844</v>
+      </c>
+      <c r="F26" t="n">
+        <v>505570</v>
+      </c>
+      <c r="G26" t="n">
+        <v>3503570</v>
+      </c>
+      <c r="H26" t="n">
+        <v>163.9900054931641</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B27" t="n">
+        <v>5321</v>
+      </c>
+      <c r="C27" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" t="n">
+        <v>6</v>
+      </c>
+      <c r="E27" t="n">
+        <v>68.34999847412109</v>
+      </c>
+      <c r="F27" t="n">
+        <v>505600</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3503600</v>
+      </c>
+      <c r="H27" t="n">
+        <v>164.1999969482422</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B28" t="n">
+        <v>5022</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" t="n">
+        <v>68.80000305175781</v>
+      </c>
+      <c r="F28" t="n">
+        <v>500630</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3500630</v>
+      </c>
+      <c r="H28" t="n">
+        <v>154.4100036621094</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B29" t="n">
+        <v>5023</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" t="n">
+        <v>3</v>
+      </c>
+      <c r="E29" t="n">
+        <v>69.62999725341797</v>
+      </c>
+      <c r="F29" t="n">
+        <v>500660</v>
+      </c>
+      <c r="G29" t="n">
+        <v>3500660</v>
+      </c>
+      <c r="H29" t="n">
+        <v>154.6199951171875</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B30" t="n">
+        <v>5023</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="n">
+        <v>4</v>
+      </c>
+      <c r="E30" t="n">
+        <v>68.80999755859375</v>
+      </c>
+      <c r="F30" t="n">
+        <v>500660</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3500660</v>
+      </c>
+      <c r="H30" t="n">
+        <v>154.6199951171875</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B31" t="n">
+        <v>5025</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" t="n">
+        <v>69.83999633789062</v>
+      </c>
+      <c r="F31" t="n">
+        <v>500720</v>
+      </c>
+      <c r="G31" t="n">
+        <v>3500720</v>
+      </c>
+      <c r="H31" t="n">
+        <v>155.0399932861328</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B32" t="n">
+        <v>5025</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="n">
+        <v>4</v>
+      </c>
+      <c r="E32" t="n">
+        <v>69.27999877929688</v>
+      </c>
+      <c r="F32" t="n">
+        <v>500720</v>
+      </c>
+      <c r="G32" t="n">
+        <v>3500720</v>
+      </c>
+      <c r="H32" t="n">
+        <v>155.0399932861328</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B33" t="n">
+        <v>5325</v>
+      </c>
+      <c r="C33" t="n">
+        <v>2</v>
+      </c>
+      <c r="D33" t="n">
+        <v>6</v>
+      </c>
+      <c r="E33" t="n">
+        <v>68.15000152587891</v>
+      </c>
+      <c r="F33" t="n">
+        <v>505720</v>
+      </c>
+      <c r="G33" t="n">
+        <v>3503720</v>
+      </c>
+      <c r="H33" t="n">
+        <v>165.0399932861328</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B34" t="n">
+        <v>5026</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" t="n">
+        <v>4</v>
+      </c>
+      <c r="E34" t="n">
+        <v>68.86000061035156</v>
+      </c>
+      <c r="F34" t="n">
+        <v>500750</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3500750</v>
+      </c>
+      <c r="H34" t="n">
+        <v>155.25</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B35" t="n">
+        <v>5028</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" t="n">
+        <v>3</v>
+      </c>
+      <c r="E35" t="n">
+        <v>69.26000213623047</v>
+      </c>
+      <c r="F35" t="n">
+        <v>500810</v>
+      </c>
+      <c r="G35" t="n">
+        <v>3500810</v>
+      </c>
+      <c r="H35" t="n">
+        <v>155.6699981689453</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B36" t="n">
+        <v>5329</v>
+      </c>
+      <c r="C36" t="n">
+        <v>2</v>
+      </c>
+      <c r="D36" t="n">
+        <v>6</v>
+      </c>
+      <c r="E36" t="n">
+        <v>69.26000213623047</v>
+      </c>
+      <c r="F36" t="n">
+        <v>505840</v>
+      </c>
+      <c r="G36" t="n">
+        <v>3503840</v>
+      </c>
+      <c r="H36" t="n">
+        <v>165.8800048828125</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B37" t="n">
+        <v>5030</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" t="n">
+        <v>68.84999847412109</v>
+      </c>
+      <c r="F37" t="n">
+        <v>500870</v>
+      </c>
+      <c r="G37" t="n">
+        <v>3500870</v>
+      </c>
+      <c r="H37" t="n">
+        <v>156.0899963378906</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B38" t="n">
+        <v>5031</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="n">
+        <v>3</v>
+      </c>
+      <c r="E38" t="n">
+        <v>69.54000091552734</v>
+      </c>
+      <c r="F38" t="n">
+        <v>500900</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3500900</v>
+      </c>
+      <c r="H38" t="n">
+        <v>156.3000030517578</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B39" t="n">
+        <v>5031</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
+        <v>4</v>
+      </c>
+      <c r="E39" t="n">
+        <v>69.54000091552734</v>
+      </c>
+      <c r="F39" t="n">
+        <v>500900</v>
+      </c>
+      <c r="G39" t="n">
+        <v>3500900</v>
+      </c>
+      <c r="H39" t="n">
+        <v>156.3000030517578</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B40" t="n">
+        <v>5332</v>
+      </c>
+      <c r="C40" t="n">
+        <v>2</v>
+      </c>
+      <c r="D40" t="n">
+        <v>7</v>
+      </c>
+      <c r="E40" t="n">
+        <v>69.23999786376953</v>
+      </c>
+      <c r="F40" t="n">
+        <v>505930</v>
+      </c>
+      <c r="G40" t="n">
+        <v>3503930</v>
+      </c>
+      <c r="H40" t="n">
+        <v>166.5099945068359</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B41" t="n">
+        <v>5033</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="n">
+        <v>3</v>
+      </c>
+      <c r="E41" t="n">
+        <v>68.84999847412109</v>
+      </c>
+      <c r="F41" t="n">
+        <v>500960</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3500960</v>
+      </c>
+      <c r="H41" t="n">
+        <v>156.7200012207031</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B42" t="n">
+        <v>5334</v>
+      </c>
+      <c r="C42" t="n">
+        <v>2</v>
+      </c>
+      <c r="D42" t="n">
+        <v>6</v>
+      </c>
+      <c r="E42" t="n">
+        <v>69.87000274658203</v>
+      </c>
+      <c r="F42" t="n">
+        <v>505990</v>
+      </c>
+      <c r="G42" t="n">
+        <v>3503990</v>
+      </c>
+      <c r="H42" t="n">
+        <v>166.9299926757812</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B43" t="n">
+        <v>5335</v>
+      </c>
+      <c r="C43" t="n">
+        <v>2</v>
+      </c>
+      <c r="D43" t="n">
+        <v>6</v>
+      </c>
+      <c r="E43" t="n">
+        <v>68.45999908447266</v>
+      </c>
+      <c r="F43" t="n">
+        <v>506020</v>
+      </c>
+      <c r="G43" t="n">
+        <v>3504020</v>
+      </c>
+      <c r="H43" t="n">
+        <v>167.1399993896484</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B44" t="n">
+        <v>5335</v>
+      </c>
+      <c r="C44" t="n">
+        <v>2</v>
+      </c>
+      <c r="D44" t="n">
+        <v>7</v>
+      </c>
+      <c r="E44" t="n">
+        <v>68.75</v>
+      </c>
+      <c r="F44" t="n">
+        <v>506020</v>
+      </c>
+      <c r="G44" t="n">
+        <v>3504020</v>
+      </c>
+      <c r="H44" t="n">
+        <v>167.1399993896484</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B45" t="n">
+        <v>5037</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" t="n">
+        <v>3</v>
+      </c>
+      <c r="E45" t="n">
+        <v>69.05999755859375</v>
+      </c>
+      <c r="F45" t="n">
+        <v>501080</v>
+      </c>
+      <c r="G45" t="n">
+        <v>3501080</v>
+      </c>
+      <c r="H45" t="n">
+        <v>157.5599975585938</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B46" t="n">
+        <v>5039</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" t="n">
+        <v>4</v>
+      </c>
+      <c r="E46" t="n">
+        <v>69.02999877929688</v>
+      </c>
+      <c r="F46" t="n">
+        <v>501140</v>
+      </c>
+      <c r="G46" t="n">
+        <v>3501140</v>
+      </c>
+      <c r="H46" t="n">
+        <v>157.9799957275391</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B47" t="n">
+        <v>5040</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" t="n">
+        <v>2</v>
+      </c>
+      <c r="E47" t="n">
+        <v>68.55000305175781</v>
+      </c>
+      <c r="F47" t="n">
+        <v>501170</v>
+      </c>
+      <c r="G47" t="n">
+        <v>3501170</v>
+      </c>
+      <c r="H47" t="n">
+        <v>158.1900024414062</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B48" t="n">
+        <v>5043</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" t="n">
+        <v>69.62000274658203</v>
+      </c>
+      <c r="F48" t="n">
+        <v>501260</v>
+      </c>
+      <c r="G48" t="n">
+        <v>3501260</v>
+      </c>
+      <c r="H48" t="n">
+        <v>158.8200073242188</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B49" t="n">
+        <v>5043</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" t="n">
+        <v>2</v>
+      </c>
+      <c r="E49" t="n">
+        <v>68.72000122070312</v>
+      </c>
+      <c r="F49" t="n">
+        <v>501260</v>
+      </c>
+      <c r="G49" t="n">
+        <v>3501260</v>
+      </c>
+      <c r="H49" t="n">
+        <v>158.8200073242188</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B50" t="n">
+        <v>5044</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" t="n">
+        <v>3</v>
+      </c>
+      <c r="E50" t="n">
+        <v>68.23000335693359</v>
+      </c>
+      <c r="F50" t="n">
+        <v>501290</v>
+      </c>
+      <c r="G50" t="n">
+        <v>3501290</v>
+      </c>
+      <c r="H50" t="n">
+        <v>159.0299987792969</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B51" t="n">
+        <v>5348</v>
+      </c>
+      <c r="C51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D51" t="n">
+        <v>8</v>
+      </c>
+      <c r="E51" t="n">
+        <v>69</v>
+      </c>
+      <c r="F51" t="n">
+        <v>506410</v>
+      </c>
+      <c r="G51" t="n">
+        <v>3504410</v>
+      </c>
+      <c r="H51" t="n">
+        <v>169.8699951171875</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B52" t="n">
+        <v>5049</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" t="n">
+        <v>2</v>
+      </c>
+      <c r="E52" t="n">
+        <v>69.30000305175781</v>
+      </c>
+      <c r="F52" t="n">
+        <v>501440</v>
+      </c>
+      <c r="G52" t="n">
+        <v>3501440</v>
+      </c>
+      <c r="H52" t="n">
+        <v>160.0800018310547</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B53" t="n">
+        <v>5049</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" t="n">
+        <v>4</v>
+      </c>
+      <c r="E53" t="n">
+        <v>68.12999725341797</v>
+      </c>
+      <c r="F53" t="n">
+        <v>501440</v>
+      </c>
+      <c r="G53" t="n">
+        <v>3501440</v>
+      </c>
+      <c r="H53" t="n">
+        <v>160.0800018310547</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B54" t="n">
+        <v>5349</v>
+      </c>
+      <c r="C54" t="n">
+        <v>2</v>
+      </c>
+      <c r="D54" t="n">
+        <v>7</v>
+      </c>
+      <c r="E54" t="n">
+        <v>68.01999664306641</v>
+      </c>
+      <c r="F54" t="n">
+        <v>506440</v>
+      </c>
+      <c r="G54" t="n">
+        <v>3504440</v>
+      </c>
+      <c r="H54" t="n">
+        <v>170.0800018310547</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B55" t="n">
+        <v>5349</v>
+      </c>
+      <c r="C55" t="n">
+        <v>2</v>
+      </c>
+      <c r="D55" t="n">
+        <v>8</v>
+      </c>
+      <c r="E55" t="n">
+        <v>68.43000030517578</v>
+      </c>
+      <c r="F55" t="n">
+        <v>506440</v>
+      </c>
+      <c r="G55" t="n">
+        <v>3504440</v>
+      </c>
+      <c r="H55" t="n">
+        <v>170.0800018310547</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B56" t="n">
+        <v>5050</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" t="n">
+        <v>3</v>
+      </c>
+      <c r="E56" t="n">
+        <v>69.77999877929688</v>
+      </c>
+      <c r="F56" t="n">
+        <v>501470</v>
+      </c>
+      <c r="G56" t="n">
+        <v>3501470</v>
+      </c>
+      <c r="H56" t="n">
+        <v>160.2899932861328</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B57" t="n">
+        <v>5050</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" t="n">
+        <v>4</v>
+      </c>
+      <c r="E57" t="n">
+        <v>68.12000274658203</v>
+      </c>
+      <c r="F57" t="n">
+        <v>501470</v>
+      </c>
+      <c r="G57" t="n">
+        <v>3501470</v>
+      </c>
+      <c r="H57" t="n">
+        <v>160.2899932861328</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B58" t="n">
+        <v>5051</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" t="n">
+        <v>2</v>
+      </c>
+      <c r="E58" t="n">
+        <v>68.69000244140625</v>
+      </c>
+      <c r="F58" t="n">
+        <v>501500</v>
+      </c>
+      <c r="G58" t="n">
+        <v>3501500</v>
+      </c>
+      <c r="H58" t="n">
+        <v>160.5</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B59" t="n">
+        <v>5051</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" t="n">
+        <v>3</v>
+      </c>
+      <c r="E59" t="n">
+        <v>68.69000244140625</v>
+      </c>
+      <c r="F59" t="n">
+        <v>501500</v>
+      </c>
+      <c r="G59" t="n">
+        <v>3501500</v>
+      </c>
+      <c r="H59" t="n">
+        <v>160.5</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B60" t="n">
+        <v>5051</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1</v>
+      </c>
+      <c r="D60" t="n">
+        <v>4</v>
+      </c>
+      <c r="E60" t="n">
+        <v>69.27999877929688</v>
+      </c>
+      <c r="F60" t="n">
+        <v>501500</v>
+      </c>
+      <c r="G60" t="n">
+        <v>3501500</v>
+      </c>
+      <c r="H60" t="n">
+        <v>160.5</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B61" t="n">
+        <v>5354</v>
+      </c>
+      <c r="C61" t="n">
+        <v>2</v>
+      </c>
+      <c r="D61" t="n">
+        <v>8</v>
+      </c>
+      <c r="E61" t="n">
+        <v>69.77999877929688</v>
+      </c>
+      <c r="F61" t="n">
+        <v>506590</v>
+      </c>
+      <c r="G61" t="n">
+        <v>3504590</v>
+      </c>
+      <c r="H61" t="n">
+        <v>171.1300048828125</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B62" t="n">
+        <v>5055</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" t="n">
+        <v>2</v>
+      </c>
+      <c r="E62" t="n">
+        <v>68.33000183105469</v>
+      </c>
+      <c r="F62" t="n">
+        <v>501620</v>
+      </c>
+      <c r="G62" t="n">
+        <v>3501620</v>
+      </c>
+      <c r="H62" t="n">
+        <v>161.3399963378906</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B63" t="n">
+        <v>5055</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" t="n">
+        <v>4</v>
+      </c>
+      <c r="E63" t="n">
+        <v>69.55000305175781</v>
+      </c>
+      <c r="F63" t="n">
+        <v>501620</v>
+      </c>
+      <c r="G63" t="n">
+        <v>3501620</v>
+      </c>
+      <c r="H63" t="n">
+        <v>161.3399963378906</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B64" t="n">
+        <v>5056</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" t="n">
+        <v>4</v>
+      </c>
+      <c r="E64" t="n">
+        <v>69.73999786376953</v>
+      </c>
+      <c r="F64" t="n">
+        <v>501650</v>
+      </c>
+      <c r="G64" t="n">
+        <v>3501650</v>
+      </c>
+      <c r="H64" t="n">
+        <v>161.5500030517578</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B65" t="n">
+        <v>5356</v>
+      </c>
+      <c r="C65" t="n">
+        <v>2</v>
+      </c>
+      <c r="D65" t="n">
+        <v>7</v>
+      </c>
+      <c r="E65" t="n">
+        <v>68.61000061035156</v>
+      </c>
+      <c r="F65" t="n">
+        <v>506650</v>
+      </c>
+      <c r="G65" t="n">
+        <v>3504650</v>
+      </c>
+      <c r="H65" t="n">
+        <v>171.5500030517578</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B66" t="n">
+        <v>5057</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" t="n">
+        <v>3</v>
+      </c>
+      <c r="E66" t="n">
+        <v>69.87000274658203</v>
+      </c>
+      <c r="F66" t="n">
+        <v>501680</v>
+      </c>
+      <c r="G66" t="n">
+        <v>3501680</v>
+      </c>
+      <c r="H66" t="n">
+        <v>161.7599945068359</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B67" t="n">
+        <v>5059</v>
+      </c>
+      <c r="C67" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" t="n">
+        <v>68.94000244140625</v>
+      </c>
+      <c r="F67" t="n">
+        <v>501740</v>
+      </c>
+      <c r="G67" t="n">
+        <v>3501740</v>
+      </c>
+      <c r="H67" t="n">
+        <v>162.1799926757812</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B68" t="n">
+        <v>5360</v>
+      </c>
+      <c r="C68" t="n">
+        <v>2</v>
+      </c>
+      <c r="D68" t="n">
+        <v>8</v>
+      </c>
+      <c r="E68" t="n">
+        <v>68.48999786376953</v>
+      </c>
+      <c r="F68" t="n">
+        <v>506770</v>
+      </c>
+      <c r="G68" t="n">
+        <v>3504770</v>
+      </c>
+      <c r="H68" t="n">
+        <v>172.3899993896484</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>5020</v>
+      </c>
+      <c r="B1" t="n">
+        <v>500569.375</v>
+      </c>
+      <c r="C1" t="n">
+        <v>3500759.25</v>
+      </c>
+      <c r="D1" t="n">
+        <v>154.25</v>
+      </c>
+      <c r="E1" t="n">
+        <v>500570</v>
+      </c>
+      <c r="F1" t="n">
+        <v>3500760</v>
+      </c>
+      <c r="G1" t="n">
+        <v>153.9900054931641</v>
+      </c>
+      <c r="H1" t="n">
+        <v>1.034456372261047</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>5035</v>
+      </c>
+      <c r="B2" t="n">
+        <v>501020.625</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3501359.25</v>
+      </c>
+      <c r="D2" t="n">
+        <v>157.6699981689453</v>
+      </c>
+      <c r="E2" t="n">
+        <v>501020</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3501360</v>
+      </c>
+      <c r="G2" t="n">
+        <v>157.1399993896484</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.130088448524475</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5360</v>
+      </c>
+      <c r="B3" t="n">
+        <v>506769.4375</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3505360.75</v>
+      </c>
+      <c r="D3" t="n">
+        <v>172.0500030517578</v>
+      </c>
+      <c r="E3" t="n">
+        <v>506770</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3505360</v>
+      </c>
+      <c r="G3" t="n">
+        <v>172.3899993896484</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.031794548034668</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -4757,4 +6644,1219 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B1" t="n">
+        <v>5302</v>
+      </c>
+      <c r="C1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E1" t="n">
+        <v>10.01000022888184</v>
+      </c>
+      <c r="F1" t="n">
+        <v>505030</v>
+      </c>
+      <c r="G1" t="n">
+        <v>3503030</v>
+      </c>
+      <c r="H1" t="n">
+        <v>160.2100067138672</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5003</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10.02999973297119</v>
+      </c>
+      <c r="F2" t="n">
+        <v>500060</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3500060</v>
+      </c>
+      <c r="H2" t="n">
+        <v>150.4199981689453</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5004</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10.01000022888184</v>
+      </c>
+      <c r="F3" t="n">
+        <v>500090</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3500090</v>
+      </c>
+      <c r="H3" t="n">
+        <v>150.6300048828125</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5304</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>10.02999973297119</v>
+      </c>
+      <c r="F4" t="n">
+        <v>505090</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3503090</v>
+      </c>
+      <c r="H4" t="n">
+        <v>160.6300048828125</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5005</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>10.01000022888184</v>
+      </c>
+      <c r="F5" t="n">
+        <v>500120</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3500120</v>
+      </c>
+      <c r="H5" t="n">
+        <v>150.8399963378906</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5305</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" t="n">
+        <v>10.02000045776367</v>
+      </c>
+      <c r="F6" t="n">
+        <v>505120</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3503120</v>
+      </c>
+      <c r="H6" t="n">
+        <v>160.8399963378906</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5008</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>10.07999992370605</v>
+      </c>
+      <c r="F7" t="n">
+        <v>500210</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3500210</v>
+      </c>
+      <c r="H7" t="n">
+        <v>151.4700012207031</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B8" t="n">
+        <v>5310</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>10.05000019073486</v>
+      </c>
+      <c r="F8" t="n">
+        <v>505270</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3503270</v>
+      </c>
+      <c r="H8" t="n">
+        <v>161.8899993896484</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B9" t="n">
+        <v>5310</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="n">
+        <v>10.01000022888184</v>
+      </c>
+      <c r="F9" t="n">
+        <v>505270</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3503270</v>
+      </c>
+      <c r="H9" t="n">
+        <v>161.8899993896484</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B10" t="n">
+        <v>5311</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10.10000038146973</v>
+      </c>
+      <c r="F10" t="n">
+        <v>505300</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3503300</v>
+      </c>
+      <c r="H10" t="n">
+        <v>162.1000061035156</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B11" t="n">
+        <v>5012</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>10.09000015258789</v>
+      </c>
+      <c r="F11" t="n">
+        <v>500330</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3500330</v>
+      </c>
+      <c r="H11" t="n">
+        <v>152.3099975585938</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B12" t="n">
+        <v>5013</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="n">
+        <v>10.09000015258789</v>
+      </c>
+      <c r="F12" t="n">
+        <v>500360</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3500360</v>
+      </c>
+      <c r="H12" t="n">
+        <v>152.5200042724609</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B13" t="n">
+        <v>5014</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="n">
+        <v>10.07999992370605</v>
+      </c>
+      <c r="F13" t="n">
+        <v>500390</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3500390</v>
+      </c>
+      <c r="H13" t="n">
+        <v>152.7299957275391</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B14" t="n">
+        <v>5316</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5</v>
+      </c>
+      <c r="E14" t="n">
+        <v>10.03999996185303</v>
+      </c>
+      <c r="F14" t="n">
+        <v>505450</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3503450</v>
+      </c>
+      <c r="H14" t="n">
+        <v>163.1499938964844</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B15" t="n">
+        <v>5019</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" t="n">
+        <v>10.05000019073486</v>
+      </c>
+      <c r="F15" t="n">
+        <v>500540</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3500540</v>
+      </c>
+      <c r="H15" t="n">
+        <v>153.7799987792969</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B16" t="n">
+        <v>5319</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>10.03999996185303</v>
+      </c>
+      <c r="F16" t="n">
+        <v>505540</v>
+      </c>
+      <c r="G16" t="n">
+        <v>3503540</v>
+      </c>
+      <c r="H16" t="n">
+        <v>163.7799987792969</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B17" t="n">
+        <v>5020</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" t="n">
+        <v>10.09000015258789</v>
+      </c>
+      <c r="F17" t="n">
+        <v>500570</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3500570</v>
+      </c>
+      <c r="H17" t="n">
+        <v>153.9900054931641</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B18" t="n">
+        <v>5323</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="n">
+        <v>7</v>
+      </c>
+      <c r="E18" t="n">
+        <v>10.03999996185303</v>
+      </c>
+      <c r="F18" t="n">
+        <v>505660</v>
+      </c>
+      <c r="G18" t="n">
+        <v>3503660</v>
+      </c>
+      <c r="H18" t="n">
+        <v>164.6199951171875</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B19" t="n">
+        <v>5324</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" t="n">
+        <v>6</v>
+      </c>
+      <c r="E19" t="n">
+        <v>10.09000015258789</v>
+      </c>
+      <c r="F19" t="n">
+        <v>505690</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3503690</v>
+      </c>
+      <c r="H19" t="n">
+        <v>164.8300018310547</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B20" t="n">
+        <v>5325</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" t="n">
+        <v>6</v>
+      </c>
+      <c r="E20" t="n">
+        <v>10.05000019073486</v>
+      </c>
+      <c r="F20" t="n">
+        <v>505720</v>
+      </c>
+      <c r="G20" t="n">
+        <v>3503720</v>
+      </c>
+      <c r="H20" t="n">
+        <v>165.0399932861328</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B21" t="n">
+        <v>5026</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" t="n">
+        <v>10.02000045776367</v>
+      </c>
+      <c r="F21" t="n">
+        <v>500750</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3500750</v>
+      </c>
+      <c r="H21" t="n">
+        <v>155.25</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B22" t="n">
+        <v>5328</v>
+      </c>
+      <c r="C22" t="n">
+        <v>2</v>
+      </c>
+      <c r="D22" t="n">
+        <v>5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>10.07999992370605</v>
+      </c>
+      <c r="F22" t="n">
+        <v>505810</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3503810</v>
+      </c>
+      <c r="H22" t="n">
+        <v>165.6699981689453</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B23" t="n">
+        <v>5328</v>
+      </c>
+      <c r="C23" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" t="n">
+        <v>8</v>
+      </c>
+      <c r="E23" t="n">
+        <v>10.06999969482422</v>
+      </c>
+      <c r="F23" t="n">
+        <v>505810</v>
+      </c>
+      <c r="G23" t="n">
+        <v>3503810</v>
+      </c>
+      <c r="H23" t="n">
+        <v>165.6699981689453</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B24" t="n">
+        <v>5330</v>
+      </c>
+      <c r="C24" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" t="n">
+        <v>5</v>
+      </c>
+      <c r="E24" t="n">
+        <v>10.05000019073486</v>
+      </c>
+      <c r="F24" t="n">
+        <v>505870</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3503870</v>
+      </c>
+      <c r="H24" t="n">
+        <v>166.0899963378906</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B25" t="n">
+        <v>5032</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="n">
+        <v>3</v>
+      </c>
+      <c r="E25" t="n">
+        <v>10.09000015258789</v>
+      </c>
+      <c r="F25" t="n">
+        <v>500930</v>
+      </c>
+      <c r="G25" t="n">
+        <v>3500930</v>
+      </c>
+      <c r="H25" t="n">
+        <v>156.5099945068359</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B26" t="n">
+        <v>5332</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" t="n">
+        <v>6</v>
+      </c>
+      <c r="E26" t="n">
+        <v>10.01000022888184</v>
+      </c>
+      <c r="F26" t="n">
+        <v>505930</v>
+      </c>
+      <c r="G26" t="n">
+        <v>3503930</v>
+      </c>
+      <c r="H26" t="n">
+        <v>166.5099945068359</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B27" t="n">
+        <v>5034</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" t="n">
+        <v>10.09000015258789</v>
+      </c>
+      <c r="F27" t="n">
+        <v>500990</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3500990</v>
+      </c>
+      <c r="H27" t="n">
+        <v>156.9299926757812</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B28" t="n">
+        <v>5336</v>
+      </c>
+      <c r="C28" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" t="n">
+        <v>7</v>
+      </c>
+      <c r="E28" t="n">
+        <v>10.0600004196167</v>
+      </c>
+      <c r="F28" t="n">
+        <v>506050</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3504050</v>
+      </c>
+      <c r="H28" t="n">
+        <v>167.3500061035156</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B29" t="n">
+        <v>5037</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" t="n">
+        <v>10.07999992370605</v>
+      </c>
+      <c r="F29" t="n">
+        <v>501080</v>
+      </c>
+      <c r="G29" t="n">
+        <v>3501080</v>
+      </c>
+      <c r="H29" t="n">
+        <v>157.5599975585938</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B30" t="n">
+        <v>5038</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" t="n">
+        <v>10.05000019073486</v>
+      </c>
+      <c r="F30" t="n">
+        <v>501110</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3501110</v>
+      </c>
+      <c r="H30" t="n">
+        <v>157.7700042724609</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B31" t="n">
+        <v>5039</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>10.02999973297119</v>
+      </c>
+      <c r="F31" t="n">
+        <v>501140</v>
+      </c>
+      <c r="G31" t="n">
+        <v>3501140</v>
+      </c>
+      <c r="H31" t="n">
+        <v>157.9799957275391</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B32" t="n">
+        <v>5039</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="n">
+        <v>4</v>
+      </c>
+      <c r="E32" t="n">
+        <v>10.05000019073486</v>
+      </c>
+      <c r="F32" t="n">
+        <v>501140</v>
+      </c>
+      <c r="G32" t="n">
+        <v>3501140</v>
+      </c>
+      <c r="H32" t="n">
+        <v>157.9799957275391</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B33" t="n">
+        <v>5040</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="n">
+        <v>3</v>
+      </c>
+      <c r="E33" t="n">
+        <v>10.07999992370605</v>
+      </c>
+      <c r="F33" t="n">
+        <v>501170</v>
+      </c>
+      <c r="G33" t="n">
+        <v>3501170</v>
+      </c>
+      <c r="H33" t="n">
+        <v>158.1900024414062</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B34" t="n">
+        <v>5345</v>
+      </c>
+      <c r="C34" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" t="n">
+        <v>8</v>
+      </c>
+      <c r="E34" t="n">
+        <v>10.01000022888184</v>
+      </c>
+      <c r="F34" t="n">
+        <v>506320</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3504320</v>
+      </c>
+      <c r="H34" t="n">
+        <v>169.2400054931641</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B35" t="n">
+        <v>5346</v>
+      </c>
+      <c r="C35" t="n">
+        <v>2</v>
+      </c>
+      <c r="D35" t="n">
+        <v>6</v>
+      </c>
+      <c r="E35" t="n">
+        <v>10.05000019073486</v>
+      </c>
+      <c r="F35" t="n">
+        <v>506350</v>
+      </c>
+      <c r="G35" t="n">
+        <v>3504350</v>
+      </c>
+      <c r="H35" t="n">
+        <v>169.4499969482422</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B36" t="n">
+        <v>5347</v>
+      </c>
+      <c r="C36" t="n">
+        <v>2</v>
+      </c>
+      <c r="D36" t="n">
+        <v>5</v>
+      </c>
+      <c r="E36" t="n">
+        <v>10.02999973297119</v>
+      </c>
+      <c r="F36" t="n">
+        <v>506380</v>
+      </c>
+      <c r="G36" t="n">
+        <v>3504380</v>
+      </c>
+      <c r="H36" t="n">
+        <v>169.6600036621094</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B37" t="n">
+        <v>5049</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>3</v>
+      </c>
+      <c r="E37" t="n">
+        <v>10.09000015258789</v>
+      </c>
+      <c r="F37" t="n">
+        <v>501440</v>
+      </c>
+      <c r="G37" t="n">
+        <v>3501440</v>
+      </c>
+      <c r="H37" t="n">
+        <v>160.0800018310547</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B38" t="n">
+        <v>5050</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="n">
+        <v>4</v>
+      </c>
+      <c r="E38" t="n">
+        <v>10.06999969482422</v>
+      </c>
+      <c r="F38" t="n">
+        <v>501470</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3501470</v>
+      </c>
+      <c r="H38" t="n">
+        <v>160.2899932861328</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B39" t="n">
+        <v>5351</v>
+      </c>
+      <c r="C39" t="n">
+        <v>2</v>
+      </c>
+      <c r="D39" t="n">
+        <v>7</v>
+      </c>
+      <c r="E39" t="n">
+        <v>10.03999996185303</v>
+      </c>
+      <c r="F39" t="n">
+        <v>506500</v>
+      </c>
+      <c r="G39" t="n">
+        <v>3504500</v>
+      </c>
+      <c r="H39" t="n">
+        <v>170.5</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B40" t="n">
+        <v>5352</v>
+      </c>
+      <c r="C40" t="n">
+        <v>2</v>
+      </c>
+      <c r="D40" t="n">
+        <v>6</v>
+      </c>
+      <c r="E40" t="n">
+        <v>10.07999992370605</v>
+      </c>
+      <c r="F40" t="n">
+        <v>506530</v>
+      </c>
+      <c r="G40" t="n">
+        <v>3504530</v>
+      </c>
+      <c r="H40" t="n">
+        <v>170.7100067138672</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B41" t="n">
+        <v>5053</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="n">
+        <v>3</v>
+      </c>
+      <c r="E41" t="n">
+        <v>10.02000045776367</v>
+      </c>
+      <c r="F41" t="n">
+        <v>501560</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3501560</v>
+      </c>
+      <c r="H41" t="n">
+        <v>160.9199981689453</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B42" t="n">
+        <v>5054</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" t="n">
+        <v>10.05000019073486</v>
+      </c>
+      <c r="F42" t="n">
+        <v>501590</v>
+      </c>
+      <c r="G42" t="n">
+        <v>3501590</v>
+      </c>
+      <c r="H42" t="n">
+        <v>161.1300048828125</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B43" t="n">
+        <v>5354</v>
+      </c>
+      <c r="C43" t="n">
+        <v>2</v>
+      </c>
+      <c r="D43" t="n">
+        <v>8</v>
+      </c>
+      <c r="E43" t="n">
+        <v>10.10000038146973</v>
+      </c>
+      <c r="F43" t="n">
+        <v>506590</v>
+      </c>
+      <c r="G43" t="n">
+        <v>3504590</v>
+      </c>
+      <c r="H43" t="n">
+        <v>171.1300048828125</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B44" t="n">
+        <v>5055</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E44" t="n">
+        <v>10.02999973297119</v>
+      </c>
+      <c r="F44" t="n">
+        <v>501620</v>
+      </c>
+      <c r="G44" t="n">
+        <v>3501620</v>
+      </c>
+      <c r="H44" t="n">
+        <v>161.3399963378906</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B45" t="n">
+        <v>5356</v>
+      </c>
+      <c r="C45" t="n">
+        <v>2</v>
+      </c>
+      <c r="D45" t="n">
+        <v>5</v>
+      </c>
+      <c r="E45" t="n">
+        <v>10.01000022888184</v>
+      </c>
+      <c r="F45" t="n">
+        <v>506650</v>
+      </c>
+      <c r="G45" t="n">
+        <v>3504650</v>
+      </c>
+      <c r="H45" t="n">
+        <v>171.5500030517578</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B46" t="n">
+        <v>5059</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" t="n">
+        <v>3</v>
+      </c>
+      <c r="E46" t="n">
+        <v>10.05000019073486</v>
+      </c>
+      <c r="F46" t="n">
+        <v>501740</v>
+      </c>
+      <c r="G46" t="n">
+        <v>3501740</v>
+      </c>
+      <c r="H46" t="n">
+        <v>162.1799926757812</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Try to put functions in different files, keep one file with all program
</commit_message>
<xml_diff>
--- a/qcdata/QCSDA.xlsx
+++ b/qcdata/QCSDA.xlsx
@@ -3302,7 +3302,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3312,80 +3312,3122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>5020</v>
+        <v>1001</v>
       </c>
       <c r="B1" t="n">
-        <v>500569.375</v>
+        <v>5001</v>
       </c>
       <c r="C1" t="n">
-        <v>3500759.25</v>
+        <v>499999.46875</v>
       </c>
       <c r="D1" t="n">
-        <v>154.25</v>
+        <v>3500000.25</v>
       </c>
       <c r="E1" t="n">
-        <v>500570</v>
+        <v>150.5200042724609</v>
       </c>
       <c r="F1" t="n">
-        <v>3500760</v>
+        <v>500000</v>
       </c>
       <c r="G1" t="n">
-        <v>153.9900054931641</v>
+        <v>3500000</v>
       </c>
       <c r="H1" t="n">
-        <v>1.034456372261047</v>
+        <v>4850.47998046875</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5035</v>
+        <v>1001</v>
       </c>
       <c r="B2" t="n">
-        <v>501020.625</v>
+        <v>5301</v>
       </c>
       <c r="C2" t="n">
-        <v>3501359.25</v>
+        <v>505000.34375</v>
       </c>
       <c r="D2" t="n">
-        <v>157.6699981689453</v>
+        <v>3503000.75</v>
       </c>
       <c r="E2" t="n">
-        <v>501020</v>
+        <v>159.4100036621094</v>
       </c>
       <c r="F2" t="n">
-        <v>3501360</v>
+        <v>505000</v>
       </c>
       <c r="G2" t="n">
-        <v>157.1399993896484</v>
+        <v>3503000</v>
       </c>
       <c r="H2" t="n">
-        <v>1.130088448524475</v>
+        <v>5141.58984375</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5002</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500030.4375</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3500040</v>
+      </c>
+      <c r="E3" t="n">
+        <v>150.3899993896484</v>
+      </c>
+      <c r="F3" t="n">
+        <v>500030</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3500040</v>
+      </c>
+      <c r="H3" t="n">
+        <v>4851.60986328125</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5302</v>
+      </c>
+      <c r="C4" t="n">
+        <v>505030.34375</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3503039.25</v>
+      </c>
+      <c r="E4" t="n">
+        <v>160.4199981689453</v>
+      </c>
+      <c r="F4" t="n">
+        <v>505030</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3503040</v>
+      </c>
+      <c r="H4" t="n">
+        <v>5141.580078125</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5003</v>
+      </c>
+      <c r="C5" t="n">
+        <v>500059.78125</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3500079.5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>150.1199951171875</v>
+      </c>
+      <c r="F5" t="n">
+        <v>500060</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3500080</v>
+      </c>
+      <c r="H5" t="n">
+        <v>4852.8798828125</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5303</v>
+      </c>
+      <c r="C6" t="n">
+        <v>505060.125</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3503080.25</v>
+      </c>
+      <c r="E6" t="n">
+        <v>160.8300018310547</v>
+      </c>
+      <c r="F6" t="n">
+        <v>505060</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3503080</v>
+      </c>
+      <c r="H6" t="n">
+        <v>5142.169921875</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5004</v>
+      </c>
+      <c r="C7" t="n">
+        <v>500089.96875</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3500119.25</v>
+      </c>
+      <c r="E7" t="n">
+        <v>150.3800048828125</v>
+      </c>
+      <c r="F7" t="n">
+        <v>500090</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3500120</v>
+      </c>
+      <c r="H7" t="n">
+        <v>4853.6201171875</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B8" t="n">
+        <v>5304</v>
+      </c>
+      <c r="C8" t="n">
+        <v>505089.40625</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3503120</v>
+      </c>
+      <c r="E8" t="n">
+        <v>160.0599975585938</v>
+      </c>
+      <c r="F8" t="n">
+        <v>505090</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3503120</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5143.93994140625</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B9" t="n">
+        <v>5005</v>
+      </c>
+      <c r="C9" t="n">
+        <v>500120.46875</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3500160</v>
+      </c>
+      <c r="E9" t="n">
+        <v>150.3500061035156</v>
+      </c>
+      <c r="F9" t="n">
+        <v>500120</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3500160</v>
+      </c>
+      <c r="H9" t="n">
+        <v>4854.64990234375</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B10" t="n">
+        <v>5305</v>
+      </c>
+      <c r="C10" t="n">
+        <v>505120.25</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3503160.75</v>
+      </c>
+      <c r="E10" t="n">
+        <v>161.1999969482422</v>
+      </c>
+      <c r="F10" t="n">
+        <v>505120</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3503160</v>
+      </c>
+      <c r="H10" t="n">
+        <v>5143.80029296875</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B11" t="n">
+        <v>5006</v>
+      </c>
+      <c r="C11" t="n">
+        <v>500149.65625</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3500199.5</v>
+      </c>
+      <c r="E11" t="n">
+        <v>151.3000030517578</v>
+      </c>
+      <c r="F11" t="n">
+        <v>500150</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3500200</v>
+      </c>
+      <c r="H11" t="n">
+        <v>4854.7001953125</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B12" t="n">
+        <v>5306</v>
+      </c>
+      <c r="C12" t="n">
+        <v>505150.65625</v>
+      </c>
+      <c r="D12" t="n">
+        <v>3503199.5</v>
+      </c>
+      <c r="E12" t="n">
+        <v>161.3899993896484</v>
+      </c>
+      <c r="F12" t="n">
+        <v>505150</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3503200</v>
+      </c>
+      <c r="H12" t="n">
+        <v>5144.60986328125</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B13" t="n">
+        <v>5007</v>
+      </c>
+      <c r="C13" t="n">
+        <v>500179.5625</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3500240.25</v>
+      </c>
+      <c r="E13" t="n">
+        <v>151.4100036621094</v>
+      </c>
+      <c r="F13" t="n">
+        <v>500180</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3500240</v>
+      </c>
+      <c r="H13" t="n">
+        <v>4855.58984375</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B14" t="n">
+        <v>5307</v>
+      </c>
+      <c r="C14" t="n">
+        <v>505179.71875</v>
+      </c>
+      <c r="D14" t="n">
+        <v>3503239.25</v>
+      </c>
+      <c r="E14" t="n">
+        <v>161.6499938964844</v>
+      </c>
+      <c r="F14" t="n">
+        <v>505180</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3503240</v>
+      </c>
+      <c r="H14" t="n">
+        <v>5145.35009765625</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B15" t="n">
+        <v>5008</v>
+      </c>
+      <c r="C15" t="n">
+        <v>500209.875</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3500280.75</v>
+      </c>
+      <c r="E15" t="n">
+        <v>150.9100036621094</v>
+      </c>
+      <c r="F15" t="n">
+        <v>500210</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3500280</v>
+      </c>
+      <c r="H15" t="n">
+        <v>4857.08984375</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B16" t="n">
+        <v>5308</v>
+      </c>
+      <c r="C16" t="n">
+        <v>505209.625</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3503279.5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>161.3600006103516</v>
+      </c>
+      <c r="F16" t="n">
+        <v>505210</v>
+      </c>
+      <c r="G16" t="n">
+        <v>3503280</v>
+      </c>
+      <c r="H16" t="n">
+        <v>5146.64013671875</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B17" t="n">
+        <v>5009</v>
+      </c>
+      <c r="C17" t="n">
+        <v>500239.5625</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3500320.25</v>
+      </c>
+      <c r="E17" t="n">
+        <v>151.3800048828125</v>
+      </c>
+      <c r="F17" t="n">
+        <v>500240</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3500320</v>
+      </c>
+      <c r="H17" t="n">
+        <v>4857.6201171875</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B18" t="n">
+        <v>5309</v>
+      </c>
+      <c r="C18" t="n">
+        <v>505240.28125</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3503320.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>161.6600036621094</v>
+      </c>
+      <c r="F18" t="n">
+        <v>505240</v>
+      </c>
+      <c r="G18" t="n">
+        <v>3503320</v>
+      </c>
+      <c r="H18" t="n">
+        <v>5147.33984375</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B19" t="n">
+        <v>5010</v>
+      </c>
+      <c r="C19" t="n">
+        <v>500269.5625</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3500360.5</v>
+      </c>
+      <c r="E19" t="n">
+        <v>152.3500061035156</v>
+      </c>
+      <c r="F19" t="n">
+        <v>500270</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3500360</v>
+      </c>
+      <c r="H19" t="n">
+        <v>4857.64990234375</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B20" t="n">
+        <v>5310</v>
+      </c>
+      <c r="C20" t="n">
+        <v>505270.03125</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3503360</v>
+      </c>
+      <c r="E20" t="n">
+        <v>161.6300048828125</v>
+      </c>
+      <c r="F20" t="n">
+        <v>505270</v>
+      </c>
+      <c r="G20" t="n">
+        <v>3503360</v>
+      </c>
+      <c r="H20" t="n">
+        <v>5148.3701171875</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B21" t="n">
+        <v>5011</v>
+      </c>
+      <c r="C21" t="n">
+        <v>500299.71875</v>
+      </c>
+      <c r="D21" t="n">
+        <v>3500400.5</v>
+      </c>
+      <c r="E21" t="n">
+        <v>152.2200012207031</v>
+      </c>
+      <c r="F21" t="n">
+        <v>500300</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3500400</v>
+      </c>
+      <c r="H21" t="n">
+        <v>4858.77978515625</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B22" t="n">
+        <v>5311</v>
+      </c>
+      <c r="C22" t="n">
+        <v>505299.9375</v>
+      </c>
+      <c r="D22" t="n">
+        <v>3503400.75</v>
+      </c>
+      <c r="E22" t="n">
+        <v>161.5299987792969</v>
+      </c>
+      <c r="F22" t="n">
+        <v>505300</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3503400</v>
+      </c>
+      <c r="H22" t="n">
+        <v>5149.47021484375</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B23" t="n">
+        <v>5012</v>
+      </c>
+      <c r="C23" t="n">
+        <v>500330.59375</v>
+      </c>
+      <c r="D23" t="n">
+        <v>3500440.75</v>
+      </c>
+      <c r="E23" t="n">
+        <v>151.8999938964844</v>
+      </c>
+      <c r="F23" t="n">
+        <v>500330</v>
+      </c>
+      <c r="G23" t="n">
+        <v>3500440</v>
+      </c>
+      <c r="H23" t="n">
+        <v>4860.10009765625</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B24" t="n">
+        <v>5312</v>
+      </c>
+      <c r="C24" t="n">
+        <v>505329.59375</v>
+      </c>
+      <c r="D24" t="n">
+        <v>3503439.5</v>
+      </c>
+      <c r="E24" t="n">
+        <v>162.7100067138672</v>
+      </c>
+      <c r="F24" t="n">
+        <v>505330</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3503440</v>
+      </c>
+      <c r="H24" t="n">
+        <v>5149.2900390625</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B25" t="n">
+        <v>5013</v>
+      </c>
+      <c r="C25" t="n">
+        <v>500359.3125</v>
+      </c>
+      <c r="D25" t="n">
+        <v>3500480</v>
+      </c>
+      <c r="E25" t="n">
+        <v>152.1499938964844</v>
+      </c>
+      <c r="F25" t="n">
+        <v>500360</v>
+      </c>
+      <c r="G25" t="n">
+        <v>3500480</v>
+      </c>
+      <c r="H25" t="n">
+        <v>4860.85009765625</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B26" t="n">
+        <v>5313</v>
+      </c>
+      <c r="C26" t="n">
+        <v>505360.5625</v>
+      </c>
+      <c r="D26" t="n">
+        <v>3503480.5</v>
+      </c>
+      <c r="E26" t="n">
+        <v>162.9199981689453</v>
+      </c>
+      <c r="F26" t="n">
+        <v>505360</v>
+      </c>
+      <c r="G26" t="n">
+        <v>3503480</v>
+      </c>
+      <c r="H26" t="n">
+        <v>5150.080078125</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B27" t="n">
+        <v>5014</v>
+      </c>
+      <c r="C27" t="n">
+        <v>500390.25</v>
+      </c>
+      <c r="D27" t="n">
+        <v>3500519.5</v>
+      </c>
+      <c r="E27" t="n">
+        <v>152.5399932861328</v>
+      </c>
+      <c r="F27" t="n">
+        <v>500390</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3500520</v>
+      </c>
+      <c r="H27" t="n">
+        <v>4861.4599609375</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B28" t="n">
+        <v>5314</v>
+      </c>
+      <c r="C28" t="n">
+        <v>505390.03125</v>
+      </c>
+      <c r="D28" t="n">
+        <v>3503520.5</v>
+      </c>
+      <c r="E28" t="n">
+        <v>162.9400024414062</v>
+      </c>
+      <c r="F28" t="n">
+        <v>505390</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3503520</v>
+      </c>
+      <c r="H28" t="n">
+        <v>5151.06005859375</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B29" t="n">
+        <v>5015</v>
+      </c>
+      <c r="C29" t="n">
+        <v>500420.03125</v>
+      </c>
+      <c r="D29" t="n">
+        <v>3500560</v>
+      </c>
+      <c r="E29" t="n">
+        <v>152.3999938964844</v>
+      </c>
+      <c r="F29" t="n">
+        <v>500420</v>
+      </c>
+      <c r="G29" t="n">
+        <v>3500560</v>
+      </c>
+      <c r="H29" t="n">
+        <v>4862.60009765625</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B30" t="n">
+        <v>5315</v>
+      </c>
+      <c r="C30" t="n">
+        <v>505419.4375</v>
+      </c>
+      <c r="D30" t="n">
+        <v>3503560.25</v>
+      </c>
+      <c r="E30" t="n">
+        <v>163.2200012207031</v>
+      </c>
+      <c r="F30" t="n">
+        <v>505420</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3503560</v>
+      </c>
+      <c r="H30" t="n">
+        <v>5151.7802734375</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B31" t="n">
+        <v>5016</v>
+      </c>
+      <c r="C31" t="n">
+        <v>500450.6875</v>
+      </c>
+      <c r="D31" t="n">
+        <v>3500599.5</v>
+      </c>
+      <c r="E31" t="n">
+        <v>153.1499938964844</v>
+      </c>
+      <c r="F31" t="n">
+        <v>500450</v>
+      </c>
+      <c r="G31" t="n">
+        <v>3500600</v>
+      </c>
+      <c r="H31" t="n">
+        <v>4862.85009765625</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B32" t="n">
+        <v>5316</v>
+      </c>
+      <c r="C32" t="n">
+        <v>505449.8125</v>
+      </c>
+      <c r="D32" t="n">
+        <v>3503599.25</v>
+      </c>
+      <c r="E32" t="n">
+        <v>163.6799926757812</v>
+      </c>
+      <c r="F32" t="n">
+        <v>505450</v>
+      </c>
+      <c r="G32" t="n">
+        <v>3503600</v>
+      </c>
+      <c r="H32" t="n">
+        <v>5152.31982421875</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B33" t="n">
+        <v>5017</v>
+      </c>
+      <c r="C33" t="n">
+        <v>500480.1875</v>
+      </c>
+      <c r="D33" t="n">
+        <v>3500639.75</v>
+      </c>
+      <c r="E33" t="n">
+        <v>153.1100006103516</v>
+      </c>
+      <c r="F33" t="n">
+        <v>500480</v>
+      </c>
+      <c r="G33" t="n">
+        <v>3500640</v>
+      </c>
+      <c r="H33" t="n">
+        <v>4863.89013671875</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B34" t="n">
+        <v>5317</v>
+      </c>
+      <c r="C34" t="n">
+        <v>505479.84375</v>
+      </c>
+      <c r="D34" t="n">
+        <v>3503640.75</v>
+      </c>
+      <c r="E34" t="n">
+        <v>163.2100067138672</v>
+      </c>
+      <c r="F34" t="n">
+        <v>505480</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3503640</v>
+      </c>
+      <c r="H34" t="n">
+        <v>5153.7900390625</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B35" t="n">
+        <v>5018</v>
+      </c>
+      <c r="C35" t="n">
+        <v>500509.3125</v>
+      </c>
+      <c r="D35" t="n">
+        <v>3500680</v>
+      </c>
+      <c r="E35" t="n">
+        <v>153.1100006103516</v>
+      </c>
+      <c r="F35" t="n">
+        <v>500510</v>
+      </c>
+      <c r="G35" t="n">
+        <v>3500680</v>
+      </c>
+      <c r="H35" t="n">
+        <v>4864.89013671875</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B36" t="n">
+        <v>5318</v>
+      </c>
+      <c r="C36" t="n">
+        <v>505510.0625</v>
+      </c>
+      <c r="D36" t="n">
+        <v>3503679.75</v>
+      </c>
+      <c r="E36" t="n">
+        <v>164.1300048828125</v>
+      </c>
+      <c r="F36" t="n">
+        <v>505510</v>
+      </c>
+      <c r="G36" t="n">
+        <v>3503680</v>
+      </c>
+      <c r="H36" t="n">
+        <v>5153.8701171875</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B37" t="n">
+        <v>5019</v>
+      </c>
+      <c r="C37" t="n">
+        <v>500540</v>
+      </c>
+      <c r="D37" t="n">
+        <v>3500720.5</v>
+      </c>
+      <c r="E37" t="n">
+        <v>153.6999969482422</v>
+      </c>
+      <c r="F37" t="n">
+        <v>500540</v>
+      </c>
+      <c r="G37" t="n">
+        <v>3500720</v>
+      </c>
+      <c r="H37" t="n">
+        <v>4865.2998046875</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B38" t="n">
+        <v>5319</v>
+      </c>
+      <c r="C38" t="n">
+        <v>505539.65625</v>
+      </c>
+      <c r="D38" t="n">
+        <v>3503720.5</v>
+      </c>
+      <c r="E38" t="n">
+        <v>163.2799987792969</v>
+      </c>
+      <c r="F38" t="n">
+        <v>505540</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3503720</v>
+      </c>
+      <c r="H38" t="n">
+        <v>5155.72021484375</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B39" t="n">
+        <v>5020</v>
+      </c>
+      <c r="C39" t="n">
+        <v>500569.375</v>
+      </c>
+      <c r="D39" t="n">
+        <v>3500759.25</v>
+      </c>
+      <c r="E39" t="n">
+        <v>154.25</v>
+      </c>
+      <c r="F39" t="n">
+        <v>500570</v>
+      </c>
+      <c r="G39" t="n">
+        <v>3500760</v>
+      </c>
+      <c r="H39" t="n">
+        <v>4865.75</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B40" t="n">
+        <v>5320</v>
+      </c>
+      <c r="C40" t="n">
+        <v>505570.46875</v>
+      </c>
+      <c r="D40" t="n">
+        <v>3503760.5</v>
+      </c>
+      <c r="E40" t="n">
+        <v>164</v>
+      </c>
+      <c r="F40" t="n">
+        <v>505570</v>
+      </c>
+      <c r="G40" t="n">
+        <v>3503760</v>
+      </c>
+      <c r="H40" t="n">
+        <v>5156</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B41" t="n">
+        <v>5021</v>
+      </c>
+      <c r="C41" t="n">
+        <v>500599.375</v>
+      </c>
+      <c r="D41" t="n">
+        <v>3500800.5</v>
+      </c>
+      <c r="E41" t="n">
+        <v>153.9900054931641</v>
+      </c>
+      <c r="F41" t="n">
+        <v>500600</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3500800</v>
+      </c>
+      <c r="H41" t="n">
+        <v>4867.01025390625</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B42" t="n">
+        <v>5321</v>
+      </c>
+      <c r="C42" t="n">
+        <v>505599.75</v>
+      </c>
+      <c r="D42" t="n">
+        <v>3503799.75</v>
+      </c>
+      <c r="E42" t="n">
+        <v>164.5</v>
+      </c>
+      <c r="F42" t="n">
+        <v>505600</v>
+      </c>
+      <c r="G42" t="n">
+        <v>3503800</v>
+      </c>
+      <c r="H42" t="n">
+        <v>5156.5</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B43" t="n">
+        <v>5022</v>
+      </c>
+      <c r="C43" t="n">
+        <v>500630.40625</v>
+      </c>
+      <c r="D43" t="n">
+        <v>3500840.25</v>
+      </c>
+      <c r="E43" t="n">
+        <v>154.8099975585938</v>
+      </c>
+      <c r="F43" t="n">
+        <v>500630</v>
+      </c>
+      <c r="G43" t="n">
+        <v>3500840</v>
+      </c>
+      <c r="H43" t="n">
+        <v>4867.18994140625</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B44" t="n">
+        <v>5322</v>
+      </c>
+      <c r="C44" t="n">
+        <v>505630.65625</v>
+      </c>
+      <c r="D44" t="n">
+        <v>3503839.75</v>
+      </c>
+      <c r="E44" t="n">
+        <v>164.1100006103516</v>
+      </c>
+      <c r="F44" t="n">
+        <v>505630</v>
+      </c>
+      <c r="G44" t="n">
+        <v>3503840</v>
+      </c>
+      <c r="H44" t="n">
+        <v>5157.89013671875</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B45" t="n">
+        <v>5023</v>
+      </c>
+      <c r="C45" t="n">
+        <v>500660.125</v>
+      </c>
+      <c r="D45" t="n">
+        <v>3500880.75</v>
+      </c>
+      <c r="E45" t="n">
+        <v>154.6600036621094</v>
+      </c>
+      <c r="F45" t="n">
+        <v>500660</v>
+      </c>
+      <c r="G45" t="n">
+        <v>3500880</v>
+      </c>
+      <c r="H45" t="n">
+        <v>4868.33984375</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B46" t="n">
+        <v>5323</v>
+      </c>
+      <c r="C46" t="n">
+        <v>505660.375</v>
+      </c>
+      <c r="D46" t="n">
+        <v>3503879.75</v>
+      </c>
+      <c r="E46" t="n">
+        <v>164.5399932861328</v>
+      </c>
+      <c r="F46" t="n">
+        <v>505660</v>
+      </c>
+      <c r="G46" t="n">
+        <v>3503880</v>
+      </c>
+      <c r="H46" t="n">
+        <v>5158.4599609375</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B47" t="n">
+        <v>5024</v>
+      </c>
+      <c r="C47" t="n">
+        <v>500690.3125</v>
+      </c>
+      <c r="D47" t="n">
+        <v>3500919.5</v>
+      </c>
+      <c r="E47" t="n">
+        <v>154.4199981689453</v>
+      </c>
+      <c r="F47" t="n">
+        <v>500690</v>
+      </c>
+      <c r="G47" t="n">
+        <v>3500920</v>
+      </c>
+      <c r="H47" t="n">
+        <v>4869.580078125</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B48" t="n">
+        <v>5324</v>
+      </c>
+      <c r="C48" t="n">
+        <v>505690.21875</v>
+      </c>
+      <c r="D48" t="n">
+        <v>3503920.5</v>
+      </c>
+      <c r="E48" t="n">
+        <v>164.9499969482422</v>
+      </c>
+      <c r="F48" t="n">
+        <v>505690</v>
+      </c>
+      <c r="G48" t="n">
+        <v>3503920</v>
+      </c>
+      <c r="H48" t="n">
+        <v>5159.0498046875</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B49" t="n">
+        <v>5025</v>
+      </c>
+      <c r="C49" t="n">
+        <v>500720.21875</v>
+      </c>
+      <c r="D49" t="n">
+        <v>3500960</v>
+      </c>
+      <c r="E49" t="n">
+        <v>155.5599975585938</v>
+      </c>
+      <c r="F49" t="n">
+        <v>500720</v>
+      </c>
+      <c r="G49" t="n">
+        <v>3500960</v>
+      </c>
+      <c r="H49" t="n">
+        <v>4869.43994140625</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B50" t="n">
+        <v>5325</v>
+      </c>
+      <c r="C50" t="n">
+        <v>505720.625</v>
+      </c>
+      <c r="D50" t="n">
+        <v>3503960.25</v>
+      </c>
+      <c r="E50" t="n">
+        <v>164.5700073242188</v>
+      </c>
+      <c r="F50" t="n">
+        <v>505720</v>
+      </c>
+      <c r="G50" t="n">
+        <v>3503960</v>
+      </c>
+      <c r="H50" t="n">
+        <v>5160.43017578125</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B51" t="n">
+        <v>5026</v>
+      </c>
+      <c r="C51" t="n">
+        <v>500750.0625</v>
+      </c>
+      <c r="D51" t="n">
+        <v>3501000.75</v>
+      </c>
+      <c r="E51" t="n">
+        <v>155.7299957275391</v>
+      </c>
+      <c r="F51" t="n">
+        <v>500750</v>
+      </c>
+      <c r="G51" t="n">
+        <v>3501000</v>
+      </c>
+      <c r="H51" t="n">
+        <v>4870.27001953125</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B52" t="n">
+        <v>5326</v>
+      </c>
+      <c r="C52" t="n">
+        <v>505749.875</v>
+      </c>
+      <c r="D52" t="n">
+        <v>3503999.75</v>
+      </c>
+      <c r="E52" t="n">
+        <v>165.3099975585938</v>
+      </c>
+      <c r="F52" t="n">
+        <v>505750</v>
+      </c>
+      <c r="G52" t="n">
+        <v>3504000</v>
+      </c>
+      <c r="H52" t="n">
+        <v>5160.68994140625</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B53" t="n">
+        <v>5027</v>
+      </c>
+      <c r="C53" t="n">
+        <v>500780.25</v>
+      </c>
+      <c r="D53" t="n">
+        <v>3501039.25</v>
+      </c>
+      <c r="E53" t="n">
+        <v>155.3699951171875</v>
+      </c>
+      <c r="F53" t="n">
+        <v>500780</v>
+      </c>
+      <c r="G53" t="n">
+        <v>3501040</v>
+      </c>
+      <c r="H53" t="n">
+        <v>4871.6298828125</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B54" t="n">
+        <v>5327</v>
+      </c>
+      <c r="C54" t="n">
+        <v>505779.90625</v>
+      </c>
+      <c r="D54" t="n">
+        <v>3504040.5</v>
+      </c>
+      <c r="E54" t="n">
+        <v>165.0399932861328</v>
+      </c>
+      <c r="F54" t="n">
+        <v>505780</v>
+      </c>
+      <c r="G54" t="n">
+        <v>3504040</v>
+      </c>
+      <c r="H54" t="n">
+        <v>5161.9599609375</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B55" t="n">
+        <v>5028</v>
+      </c>
+      <c r="C55" t="n">
+        <v>500809.5</v>
+      </c>
+      <c r="D55" t="n">
+        <v>3501079.75</v>
+      </c>
+      <c r="E55" t="n">
+        <v>155.3699951171875</v>
+      </c>
+      <c r="F55" t="n">
+        <v>500810</v>
+      </c>
+      <c r="G55" t="n">
+        <v>3501080</v>
+      </c>
+      <c r="H55" t="n">
+        <v>4872.6298828125</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B56" t="n">
+        <v>5328</v>
+      </c>
+      <c r="C56" t="n">
+        <v>505809.90625</v>
+      </c>
+      <c r="D56" t="n">
+        <v>3504080.25</v>
+      </c>
+      <c r="E56" t="n">
+        <v>165.6100006103516</v>
+      </c>
+      <c r="F56" t="n">
+        <v>505810</v>
+      </c>
+      <c r="G56" t="n">
+        <v>3504080</v>
+      </c>
+      <c r="H56" t="n">
+        <v>5162.39013671875</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B57" t="n">
+        <v>5029</v>
+      </c>
+      <c r="C57" t="n">
+        <v>500840.0625</v>
+      </c>
+      <c r="D57" t="n">
+        <v>3501119.5</v>
+      </c>
+      <c r="E57" t="n">
+        <v>155.9199981689453</v>
+      </c>
+      <c r="F57" t="n">
+        <v>500840</v>
+      </c>
+      <c r="G57" t="n">
+        <v>3501120</v>
+      </c>
+      <c r="H57" t="n">
+        <v>4873.080078125</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B58" t="n">
+        <v>5329</v>
+      </c>
+      <c r="C58" t="n">
+        <v>505839.84375</v>
+      </c>
+      <c r="D58" t="n">
+        <v>3504119.25</v>
+      </c>
+      <c r="E58" t="n">
+        <v>165.7100067138672</v>
+      </c>
+      <c r="F58" t="n">
+        <v>505840</v>
+      </c>
+      <c r="G58" t="n">
+        <v>3504120</v>
+      </c>
+      <c r="H58" t="n">
+        <v>5163.2900390625</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B59" t="n">
+        <v>5030</v>
+      </c>
+      <c r="C59" t="n">
+        <v>500869.875</v>
+      </c>
+      <c r="D59" t="n">
+        <v>3501159.5</v>
+      </c>
+      <c r="E59" t="n">
+        <v>156.4199981689453</v>
+      </c>
+      <c r="F59" t="n">
+        <v>500870</v>
+      </c>
+      <c r="G59" t="n">
+        <v>3501160</v>
+      </c>
+      <c r="H59" t="n">
+        <v>4873.580078125</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B60" t="n">
+        <v>5330</v>
+      </c>
+      <c r="C60" t="n">
+        <v>505870.34375</v>
+      </c>
+      <c r="D60" t="n">
+        <v>3504160.5</v>
+      </c>
+      <c r="E60" t="n">
+        <v>166.5500030517578</v>
+      </c>
+      <c r="F60" t="n">
+        <v>505870</v>
+      </c>
+      <c r="G60" t="n">
+        <v>3504160</v>
+      </c>
+      <c r="H60" t="n">
+        <v>5163.4501953125</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B61" t="n">
+        <v>5031</v>
+      </c>
+      <c r="C61" t="n">
+        <v>500900.03125</v>
+      </c>
+      <c r="D61" t="n">
+        <v>3501199.75</v>
+      </c>
+      <c r="E61" t="n">
+        <v>156.5800018310547</v>
+      </c>
+      <c r="F61" t="n">
+        <v>500900</v>
+      </c>
+      <c r="G61" t="n">
+        <v>3501200</v>
+      </c>
+      <c r="H61" t="n">
+        <v>4874.419921875</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B62" t="n">
+        <v>5331</v>
+      </c>
+      <c r="C62" t="n">
+        <v>505900</v>
+      </c>
+      <c r="D62" t="n">
+        <v>3504199.75</v>
+      </c>
+      <c r="E62" t="n">
+        <v>166.1900024414062</v>
+      </c>
+      <c r="F62" t="n">
+        <v>505900</v>
+      </c>
+      <c r="G62" t="n">
+        <v>3504200</v>
+      </c>
+      <c r="H62" t="n">
+        <v>5164.81005859375</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B63" t="n">
+        <v>5032</v>
+      </c>
+      <c r="C63" t="n">
+        <v>500929.40625</v>
+      </c>
+      <c r="D63" t="n">
+        <v>3501240.25</v>
+      </c>
+      <c r="E63" t="n">
+        <v>156.6399993896484</v>
+      </c>
+      <c r="F63" t="n">
+        <v>500930</v>
+      </c>
+      <c r="G63" t="n">
+        <v>3501240</v>
+      </c>
+      <c r="H63" t="n">
+        <v>4875.35986328125</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B64" t="n">
+        <v>5332</v>
+      </c>
+      <c r="C64" t="n">
+        <v>505929.65625</v>
+      </c>
+      <c r="D64" t="n">
+        <v>3504240.5</v>
+      </c>
+      <c r="E64" t="n">
+        <v>166.6799926757812</v>
+      </c>
+      <c r="F64" t="n">
+        <v>505930</v>
+      </c>
+      <c r="G64" t="n">
+        <v>3504240</v>
+      </c>
+      <c r="H64" t="n">
+        <v>5165.31982421875</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B65" t="n">
+        <v>5033</v>
+      </c>
+      <c r="C65" t="n">
+        <v>500959.9375</v>
+      </c>
+      <c r="D65" t="n">
+        <v>3501280.5</v>
+      </c>
+      <c r="E65" t="n">
+        <v>156.2700042724609</v>
+      </c>
+      <c r="F65" t="n">
+        <v>500960</v>
+      </c>
+      <c r="G65" t="n">
+        <v>3501280</v>
+      </c>
+      <c r="H65" t="n">
+        <v>4876.72998046875</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B66" t="n">
+        <v>5333</v>
+      </c>
+      <c r="C66" t="n">
+        <v>505960.1875</v>
+      </c>
+      <c r="D66" t="n">
+        <v>3504279.75</v>
+      </c>
+      <c r="E66" t="n">
+        <v>166.7200012207031</v>
+      </c>
+      <c r="F66" t="n">
+        <v>505960</v>
+      </c>
+      <c r="G66" t="n">
+        <v>3504280</v>
+      </c>
+      <c r="H66" t="n">
+        <v>5166.27978515625</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B67" t="n">
+        <v>5034</v>
+      </c>
+      <c r="C67" t="n">
+        <v>500990.28125</v>
+      </c>
+      <c r="D67" t="n">
+        <v>3501319.5</v>
+      </c>
+      <c r="E67" t="n">
+        <v>156.6999969482422</v>
+      </c>
+      <c r="F67" t="n">
+        <v>500990</v>
+      </c>
+      <c r="G67" t="n">
+        <v>3501320</v>
+      </c>
+      <c r="H67" t="n">
+        <v>4877.2998046875</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B68" t="n">
+        <v>5334</v>
+      </c>
+      <c r="C68" t="n">
+        <v>505990.6875</v>
+      </c>
+      <c r="D68" t="n">
+        <v>3504320.25</v>
+      </c>
+      <c r="E68" t="n">
+        <v>167.0200042724609</v>
+      </c>
+      <c r="F68" t="n">
+        <v>505990</v>
+      </c>
+      <c r="G68" t="n">
+        <v>3504320</v>
+      </c>
+      <c r="H68" t="n">
+        <v>5166.97998046875</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B69" t="n">
+        <v>5035</v>
+      </c>
+      <c r="C69" t="n">
+        <v>501020.625</v>
+      </c>
+      <c r="D69" t="n">
+        <v>3501359.25</v>
+      </c>
+      <c r="E69" t="n">
+        <v>157.6699981689453</v>
+      </c>
+      <c r="F69" t="n">
+        <v>501020</v>
+      </c>
+      <c r="G69" t="n">
+        <v>3501360</v>
+      </c>
+      <c r="H69" t="n">
+        <v>4877.330078125</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B70" t="n">
+        <v>5335</v>
+      </c>
+      <c r="C70" t="n">
+        <v>506019.4375</v>
+      </c>
+      <c r="D70" t="n">
+        <v>3504359.75</v>
+      </c>
+      <c r="E70" t="n">
+        <v>167.0500030517578</v>
+      </c>
+      <c r="F70" t="n">
+        <v>506020</v>
+      </c>
+      <c r="G70" t="n">
+        <v>3504360</v>
+      </c>
+      <c r="H70" t="n">
+        <v>5167.9501953125</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B71" t="n">
+        <v>5036</v>
+      </c>
+      <c r="C71" t="n">
+        <v>501050.625</v>
+      </c>
+      <c r="D71" t="n">
+        <v>3501400.25</v>
+      </c>
+      <c r="E71" t="n">
+        <v>156.7899932861328</v>
+      </c>
+      <c r="F71" t="n">
+        <v>501050</v>
+      </c>
+      <c r="G71" t="n">
+        <v>3501400</v>
+      </c>
+      <c r="H71" t="n">
+        <v>4879.2099609375</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B72" t="n">
+        <v>5336</v>
+      </c>
+      <c r="C72" t="n">
+        <v>506049.53125</v>
+      </c>
+      <c r="D72" t="n">
+        <v>3504400.25</v>
+      </c>
+      <c r="E72" t="n">
+        <v>167.8699951171875</v>
+      </c>
+      <c r="F72" t="n">
+        <v>506050</v>
+      </c>
+      <c r="G72" t="n">
+        <v>3504400</v>
+      </c>
+      <c r="H72" t="n">
+        <v>5168.1298828125</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B73" t="n">
+        <v>5037</v>
+      </c>
+      <c r="C73" t="n">
+        <v>501080.65625</v>
+      </c>
+      <c r="D73" t="n">
+        <v>3501439.75</v>
+      </c>
+      <c r="E73" t="n">
+        <v>158.0700073242188</v>
+      </c>
+      <c r="F73" t="n">
+        <v>501080</v>
+      </c>
+      <c r="G73" t="n">
+        <v>3501440</v>
+      </c>
+      <c r="H73" t="n">
+        <v>4878.93017578125</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B74" t="n">
+        <v>5337</v>
+      </c>
+      <c r="C74" t="n">
+        <v>506080.125</v>
+      </c>
+      <c r="D74" t="n">
+        <v>3504440.75</v>
+      </c>
+      <c r="E74" t="n">
+        <v>167.3899993896484</v>
+      </c>
+      <c r="F74" t="n">
+        <v>506080</v>
+      </c>
+      <c r="G74" t="n">
+        <v>3504440</v>
+      </c>
+      <c r="H74" t="n">
+        <v>5169.60986328125</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B75" t="n">
+        <v>5038</v>
+      </c>
+      <c r="C75" t="n">
+        <v>501109.625</v>
+      </c>
+      <c r="D75" t="n">
+        <v>3501479.5</v>
+      </c>
+      <c r="E75" t="n">
+        <v>157.4799957275391</v>
+      </c>
+      <c r="F75" t="n">
+        <v>501110</v>
+      </c>
+      <c r="G75" t="n">
+        <v>3501480</v>
+      </c>
+      <c r="H75" t="n">
+        <v>4880.52001953125</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B76" t="n">
+        <v>5338</v>
+      </c>
+      <c r="C76" t="n">
+        <v>506109.40625</v>
+      </c>
+      <c r="D76" t="n">
+        <v>3504480.5</v>
+      </c>
+      <c r="E76" t="n">
+        <v>168.1100006103516</v>
+      </c>
+      <c r="F76" t="n">
+        <v>506110</v>
+      </c>
+      <c r="G76" t="n">
+        <v>3504480</v>
+      </c>
+      <c r="H76" t="n">
+        <v>5169.89013671875</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B77" t="n">
+        <v>5039</v>
+      </c>
+      <c r="C77" t="n">
+        <v>501139.71875</v>
+      </c>
+      <c r="D77" t="n">
+        <v>3501519.5</v>
+      </c>
+      <c r="E77" t="n">
+        <v>157.9900054931641</v>
+      </c>
+      <c r="F77" t="n">
+        <v>501140</v>
+      </c>
+      <c r="G77" t="n">
+        <v>3501520</v>
+      </c>
+      <c r="H77" t="n">
+        <v>4881.01025390625</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B78" t="n">
+        <v>5339</v>
+      </c>
+      <c r="C78" t="n">
+        <v>506140.4375</v>
+      </c>
+      <c r="D78" t="n">
+        <v>3504520</v>
+      </c>
+      <c r="E78" t="n">
+        <v>168.0599975585938</v>
+      </c>
+      <c r="F78" t="n">
+        <v>506140</v>
+      </c>
+      <c r="G78" t="n">
+        <v>3504520</v>
+      </c>
+      <c r="H78" t="n">
+        <v>5170.93994140625</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B79" t="n">
+        <v>5040</v>
+      </c>
+      <c r="C79" t="n">
+        <v>501169.40625</v>
+      </c>
+      <c r="D79" t="n">
+        <v>3501560.5</v>
+      </c>
+      <c r="E79" t="n">
+        <v>158.4100036621094</v>
+      </c>
+      <c r="F79" t="n">
+        <v>501170</v>
+      </c>
+      <c r="G79" t="n">
+        <v>3501560</v>
+      </c>
+      <c r="H79" t="n">
+        <v>4881.58984375</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B80" t="n">
+        <v>5340</v>
+      </c>
+      <c r="C80" t="n">
+        <v>506169.8125</v>
+      </c>
+      <c r="D80" t="n">
+        <v>3504559.75</v>
+      </c>
+      <c r="E80" t="n">
+        <v>167.6999969482422</v>
+      </c>
+      <c r="F80" t="n">
+        <v>506170</v>
+      </c>
+      <c r="G80" t="n">
+        <v>3504560</v>
+      </c>
+      <c r="H80" t="n">
+        <v>5172.2998046875</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B81" t="n">
+        <v>5041</v>
+      </c>
+      <c r="C81" t="n">
+        <v>501199.46875</v>
+      </c>
+      <c r="D81" t="n">
+        <v>3501599.25</v>
+      </c>
+      <c r="E81" t="n">
+        <v>158.8500061035156</v>
+      </c>
+      <c r="F81" t="n">
+        <v>501200</v>
+      </c>
+      <c r="G81" t="n">
+        <v>3501600</v>
+      </c>
+      <c r="H81" t="n">
+        <v>4882.14990234375</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B82" t="n">
+        <v>5341</v>
+      </c>
+      <c r="C82" t="n">
+        <v>506199.53125</v>
+      </c>
+      <c r="D82" t="n">
+        <v>3504600</v>
+      </c>
+      <c r="E82" t="n">
+        <v>168.9299926757812</v>
+      </c>
+      <c r="F82" t="n">
+        <v>506200</v>
+      </c>
+      <c r="G82" t="n">
+        <v>3504600</v>
+      </c>
+      <c r="H82" t="n">
+        <v>5172.06982421875</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B83" t="n">
+        <v>5042</v>
+      </c>
+      <c r="C83" t="n">
+        <v>501229.375</v>
+      </c>
+      <c r="D83" t="n">
+        <v>3501639.75</v>
+      </c>
+      <c r="E83" t="n">
+        <v>158.1300048828125</v>
+      </c>
+      <c r="F83" t="n">
+        <v>501230</v>
+      </c>
+      <c r="G83" t="n">
+        <v>3501640</v>
+      </c>
+      <c r="H83" t="n">
+        <v>4883.8701171875</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B84" t="n">
+        <v>5342</v>
+      </c>
+      <c r="C84" t="n">
+        <v>506230.28125</v>
+      </c>
+      <c r="D84" t="n">
+        <v>3504639.5</v>
+      </c>
+      <c r="E84" t="n">
+        <v>169.0299987792969</v>
+      </c>
+      <c r="F84" t="n">
+        <v>506230</v>
+      </c>
+      <c r="G84" t="n">
+        <v>3504640</v>
+      </c>
+      <c r="H84" t="n">
+        <v>5172.97021484375</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B85" t="n">
+        <v>5043</v>
+      </c>
+      <c r="C85" t="n">
+        <v>501259.40625</v>
+      </c>
+      <c r="D85" t="n">
+        <v>3501680.25</v>
+      </c>
+      <c r="E85" t="n">
+        <v>159.3099975585938</v>
+      </c>
+      <c r="F85" t="n">
+        <v>501260</v>
+      </c>
+      <c r="G85" t="n">
+        <v>3501680</v>
+      </c>
+      <c r="H85" t="n">
+        <v>4883.68994140625</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B86" t="n">
+        <v>5343</v>
+      </c>
+      <c r="C86" t="n">
+        <v>506260.15625</v>
+      </c>
+      <c r="D86" t="n">
+        <v>3504680</v>
+      </c>
+      <c r="E86" t="n">
+        <v>168.2299957275391</v>
+      </c>
+      <c r="F86" t="n">
+        <v>506260</v>
+      </c>
+      <c r="G86" t="n">
+        <v>3504680</v>
+      </c>
+      <c r="H86" t="n">
+        <v>5174.77001953125</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B87" t="n">
+        <v>5044</v>
+      </c>
+      <c r="C87" t="n">
+        <v>501289.53125</v>
+      </c>
+      <c r="D87" t="n">
+        <v>3501719.5</v>
+      </c>
+      <c r="E87" t="n">
+        <v>159.0599975585938</v>
+      </c>
+      <c r="F87" t="n">
+        <v>501290</v>
+      </c>
+      <c r="G87" t="n">
+        <v>3501720</v>
+      </c>
+      <c r="H87" t="n">
+        <v>4884.93994140625</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B88" t="n">
+        <v>5344</v>
+      </c>
+      <c r="C88" t="n">
+        <v>506290.21875</v>
+      </c>
+      <c r="D88" t="n">
+        <v>3504719.25</v>
+      </c>
+      <c r="E88" t="n">
+        <v>169.2100067138672</v>
+      </c>
+      <c r="F88" t="n">
+        <v>506290</v>
+      </c>
+      <c r="G88" t="n">
+        <v>3504720</v>
+      </c>
+      <c r="H88" t="n">
+        <v>5174.7900390625</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B89" t="n">
+        <v>5045</v>
+      </c>
+      <c r="C89" t="n">
+        <v>501320</v>
+      </c>
+      <c r="D89" t="n">
+        <v>3501759.5</v>
+      </c>
+      <c r="E89" t="n">
+        <v>159.1000061035156</v>
+      </c>
+      <c r="F89" t="n">
+        <v>501320</v>
+      </c>
+      <c r="G89" t="n">
+        <v>3501760</v>
+      </c>
+      <c r="H89" t="n">
+        <v>4885.89990234375</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B90" t="n">
+        <v>5345</v>
+      </c>
+      <c r="C90" t="n">
+        <v>506319.6875</v>
+      </c>
+      <c r="D90" t="n">
+        <v>3504759.5</v>
+      </c>
+      <c r="E90" t="n">
+        <v>169.4199981689453</v>
+      </c>
+      <c r="F90" t="n">
+        <v>506320</v>
+      </c>
+      <c r="G90" t="n">
+        <v>3504760</v>
+      </c>
+      <c r="H90" t="n">
+        <v>5175.580078125</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B91" t="n">
+        <v>5046</v>
+      </c>
+      <c r="C91" t="n">
+        <v>501350.46875</v>
+      </c>
+      <c r="D91" t="n">
+        <v>3501799.75</v>
+      </c>
+      <c r="E91" t="n">
+        <v>159.7700042724609</v>
+      </c>
+      <c r="F91" t="n">
+        <v>501350</v>
+      </c>
+      <c r="G91" t="n">
+        <v>3501800</v>
+      </c>
+      <c r="H91" t="n">
+        <v>4886.22998046875</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B92" t="n">
+        <v>5346</v>
+      </c>
+      <c r="C92" t="n">
+        <v>506350.4375</v>
+      </c>
+      <c r="D92" t="n">
+        <v>3504800.75</v>
+      </c>
+      <c r="E92" t="n">
+        <v>169.5399932861328</v>
+      </c>
+      <c r="F92" t="n">
+        <v>506350</v>
+      </c>
+      <c r="G92" t="n">
+        <v>3504800</v>
+      </c>
+      <c r="H92" t="n">
+        <v>5176.4599609375</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B93" t="n">
+        <v>5047</v>
+      </c>
+      <c r="C93" t="n">
+        <v>501380.625</v>
+      </c>
+      <c r="D93" t="n">
+        <v>3501840</v>
+      </c>
+      <c r="E93" t="n">
+        <v>159.8200073242188</v>
+      </c>
+      <c r="F93" t="n">
+        <v>501380</v>
+      </c>
+      <c r="G93" t="n">
+        <v>3501840</v>
+      </c>
+      <c r="H93" t="n">
+        <v>4887.18017578125</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B94" t="n">
+        <v>5347</v>
+      </c>
+      <c r="C94" t="n">
+        <v>506379.3125</v>
+      </c>
+      <c r="D94" t="n">
+        <v>3504839.5</v>
+      </c>
+      <c r="E94" t="n">
+        <v>169.3899993896484</v>
+      </c>
+      <c r="F94" t="n">
+        <v>506380</v>
+      </c>
+      <c r="G94" t="n">
+        <v>3504840</v>
+      </c>
+      <c r="H94" t="n">
+        <v>5177.60986328125</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B95" t="n">
+        <v>5048</v>
+      </c>
+      <c r="C95" t="n">
+        <v>501410.1875</v>
+      </c>
+      <c r="D95" t="n">
+        <v>3501880</v>
+      </c>
+      <c r="E95" t="n">
+        <v>160.2799987792969</v>
+      </c>
+      <c r="F95" t="n">
+        <v>501410</v>
+      </c>
+      <c r="G95" t="n">
+        <v>3501880</v>
+      </c>
+      <c r="H95" t="n">
+        <v>4887.72021484375</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B96" t="n">
+        <v>5348</v>
+      </c>
+      <c r="C96" t="n">
+        <v>506409.3125</v>
+      </c>
+      <c r="D96" t="n">
+        <v>3504880.25</v>
+      </c>
+      <c r="E96" t="n">
+        <v>169.7799987792969</v>
+      </c>
+      <c r="F96" t="n">
+        <v>506410</v>
+      </c>
+      <c r="G96" t="n">
+        <v>3504880</v>
+      </c>
+      <c r="H96" t="n">
+        <v>5178.22021484375</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B97" t="n">
+        <v>5049</v>
+      </c>
+      <c r="C97" t="n">
+        <v>501439.4375</v>
+      </c>
+      <c r="D97" t="n">
+        <v>3501920</v>
+      </c>
+      <c r="E97" t="n">
+        <v>160.2400054931641</v>
+      </c>
+      <c r="F97" t="n">
+        <v>501440</v>
+      </c>
+      <c r="G97" t="n">
+        <v>3501920</v>
+      </c>
+      <c r="H97" t="n">
+        <v>4888.76025390625</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B98" t="n">
+        <v>5349</v>
+      </c>
+      <c r="C98" t="n">
+        <v>506439.4375</v>
+      </c>
+      <c r="D98" t="n">
+        <v>3504920.25</v>
+      </c>
+      <c r="E98" t="n">
+        <v>170.4799957275391</v>
+      </c>
+      <c r="F98" t="n">
+        <v>506440</v>
+      </c>
+      <c r="G98" t="n">
+        <v>3504920</v>
+      </c>
+      <c r="H98" t="n">
+        <v>5178.52001953125</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B99" t="n">
+        <v>5050</v>
+      </c>
+      <c r="C99" t="n">
+        <v>501469.8125</v>
+      </c>
+      <c r="D99" t="n">
+        <v>3501960.5</v>
+      </c>
+      <c r="E99" t="n">
+        <v>160.0099945068359</v>
+      </c>
+      <c r="F99" t="n">
+        <v>501470</v>
+      </c>
+      <c r="G99" t="n">
+        <v>3501960</v>
+      </c>
+      <c r="H99" t="n">
+        <v>4889.990234375</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B100" t="n">
+        <v>5350</v>
+      </c>
+      <c r="C100" t="n">
+        <v>506469.625</v>
+      </c>
+      <c r="D100" t="n">
+        <v>3504959.75</v>
+      </c>
+      <c r="E100" t="n">
+        <v>170.1699981689453</v>
+      </c>
+      <c r="F100" t="n">
+        <v>506470</v>
+      </c>
+      <c r="G100" t="n">
+        <v>3504960</v>
+      </c>
+      <c r="H100" t="n">
+        <v>5179.830078125</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B101" t="n">
+        <v>5051</v>
+      </c>
+      <c r="C101" t="n">
+        <v>501499.78125</v>
+      </c>
+      <c r="D101" t="n">
+        <v>3502000.5</v>
+      </c>
+      <c r="E101" t="n">
+        <v>160.5700073242188</v>
+      </c>
+      <c r="F101" t="n">
+        <v>501500</v>
+      </c>
+      <c r="G101" t="n">
+        <v>3502000</v>
+      </c>
+      <c r="H101" t="n">
+        <v>4890.43017578125</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B102" t="n">
+        <v>5351</v>
+      </c>
+      <c r="C102" t="n">
+        <v>506499.65625</v>
+      </c>
+      <c r="D102" t="n">
+        <v>3504999.5</v>
+      </c>
+      <c r="E102" t="n">
+        <v>170.4299926757812</v>
+      </c>
+      <c r="F102" t="n">
+        <v>506500</v>
+      </c>
+      <c r="G102" t="n">
+        <v>3505000</v>
+      </c>
+      <c r="H102" t="n">
+        <v>5180.56982421875</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B103" t="n">
+        <v>5052</v>
+      </c>
+      <c r="C103" t="n">
+        <v>501529.84375</v>
+      </c>
+      <c r="D103" t="n">
+        <v>3502039.25</v>
+      </c>
+      <c r="E103" t="n">
+        <v>160.2200012207031</v>
+      </c>
+      <c r="F103" t="n">
+        <v>501530</v>
+      </c>
+      <c r="G103" t="n">
+        <v>3502040</v>
+      </c>
+      <c r="H103" t="n">
+        <v>4891.7802734375</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B104" t="n">
+        <v>5352</v>
+      </c>
+      <c r="C104" t="n">
+        <v>506529.875</v>
+      </c>
+      <c r="D104" t="n">
+        <v>3505039.75</v>
+      </c>
+      <c r="E104" t="n">
+        <v>171</v>
+      </c>
+      <c r="F104" t="n">
+        <v>506530</v>
+      </c>
+      <c r="G104" t="n">
+        <v>3505040</v>
+      </c>
+      <c r="H104" t="n">
+        <v>5181</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B105" t="n">
+        <v>5053</v>
+      </c>
+      <c r="C105" t="n">
+        <v>501560.1875</v>
+      </c>
+      <c r="D105" t="n">
+        <v>3502080.5</v>
+      </c>
+      <c r="E105" t="n">
+        <v>160.3600006103516</v>
+      </c>
+      <c r="F105" t="n">
+        <v>501560</v>
+      </c>
+      <c r="G105" t="n">
+        <v>3502080</v>
+      </c>
+      <c r="H105" t="n">
+        <v>4892.64013671875</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B106" t="n">
+        <v>5353</v>
+      </c>
+      <c r="C106" t="n">
+        <v>506560.40625</v>
+      </c>
+      <c r="D106" t="n">
+        <v>3505079.75</v>
+      </c>
+      <c r="E106" t="n">
+        <v>170.8399963378906</v>
+      </c>
+      <c r="F106" t="n">
+        <v>506560</v>
+      </c>
+      <c r="G106" t="n">
+        <v>3505080</v>
+      </c>
+      <c r="H106" t="n">
+        <v>5182.16015625</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B107" t="n">
+        <v>5054</v>
+      </c>
+      <c r="C107" t="n">
+        <v>501589.6875</v>
+      </c>
+      <c r="D107" t="n">
+        <v>3502120.75</v>
+      </c>
+      <c r="E107" t="n">
+        <v>160.5700073242188</v>
+      </c>
+      <c r="F107" t="n">
+        <v>501590</v>
+      </c>
+      <c r="G107" t="n">
+        <v>3502120</v>
+      </c>
+      <c r="H107" t="n">
+        <v>4893.43017578125</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B108" t="n">
+        <v>5354</v>
+      </c>
+      <c r="C108" t="n">
+        <v>506590.46875</v>
+      </c>
+      <c r="D108" t="n">
+        <v>3505120.25</v>
+      </c>
+      <c r="E108" t="n">
+        <v>171.6999969482422</v>
+      </c>
+      <c r="F108" t="n">
+        <v>506590</v>
+      </c>
+      <c r="G108" t="n">
+        <v>3505120</v>
+      </c>
+      <c r="H108" t="n">
+        <v>5182.2998046875</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B109" t="n">
+        <v>5055</v>
+      </c>
+      <c r="C109" t="n">
+        <v>501620.34375</v>
+      </c>
+      <c r="D109" t="n">
+        <v>3502159.75</v>
+      </c>
+      <c r="E109" t="n">
+        <v>161.3699951171875</v>
+      </c>
+      <c r="F109" t="n">
+        <v>501620</v>
+      </c>
+      <c r="G109" t="n">
+        <v>3502160</v>
+      </c>
+      <c r="H109" t="n">
+        <v>4893.6298828125</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B110" t="n">
+        <v>5355</v>
+      </c>
+      <c r="C110" t="n">
+        <v>506620.46875</v>
+      </c>
+      <c r="D110" t="n">
+        <v>3505160.75</v>
+      </c>
+      <c r="E110" t="n">
+        <v>171.8300018310547</v>
+      </c>
+      <c r="F110" t="n">
+        <v>506620</v>
+      </c>
+      <c r="G110" t="n">
+        <v>3505160</v>
+      </c>
+      <c r="H110" t="n">
+        <v>5183.169921875</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B111" t="n">
+        <v>5056</v>
+      </c>
+      <c r="C111" t="n">
+        <v>501649.5625</v>
+      </c>
+      <c r="D111" t="n">
+        <v>3502200.75</v>
+      </c>
+      <c r="E111" t="n">
+        <v>161.4100036621094</v>
+      </c>
+      <c r="F111" t="n">
+        <v>501650</v>
+      </c>
+      <c r="G111" t="n">
+        <v>3502200</v>
+      </c>
+      <c r="H111" t="n">
+        <v>4894.58984375</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B112" t="n">
+        <v>5356</v>
+      </c>
+      <c r="C112" t="n">
+        <v>506649.375</v>
+      </c>
+      <c r="D112" t="n">
+        <v>3505200.5</v>
+      </c>
+      <c r="E112" t="n">
+        <v>172.0099945068359</v>
+      </c>
+      <c r="F112" t="n">
+        <v>506650</v>
+      </c>
+      <c r="G112" t="n">
+        <v>3505200</v>
+      </c>
+      <c r="H112" t="n">
+        <v>5183.990234375</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B113" t="n">
+        <v>5057</v>
+      </c>
+      <c r="C113" t="n">
+        <v>501680.15625</v>
+      </c>
+      <c r="D113" t="n">
+        <v>3502239.5</v>
+      </c>
+      <c r="E113" t="n">
+        <v>161.4700012207031</v>
+      </c>
+      <c r="F113" t="n">
+        <v>501680</v>
+      </c>
+      <c r="G113" t="n">
+        <v>3502240</v>
+      </c>
+      <c r="H113" t="n">
+        <v>4895.52978515625</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B114" t="n">
+        <v>5357</v>
+      </c>
+      <c r="C114" t="n">
+        <v>506680.28125</v>
+      </c>
+      <c r="D114" t="n">
+        <v>3505239.75</v>
+      </c>
+      <c r="E114" t="n">
+        <v>172.25</v>
+      </c>
+      <c r="F114" t="n">
+        <v>506680</v>
+      </c>
+      <c r="G114" t="n">
+        <v>3505240</v>
+      </c>
+      <c r="H114" t="n">
+        <v>5184.75</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B115" t="n">
+        <v>5058</v>
+      </c>
+      <c r="C115" t="n">
+        <v>501709.46875</v>
+      </c>
+      <c r="D115" t="n">
+        <v>3502280.5</v>
+      </c>
+      <c r="E115" t="n">
+        <v>162.4400024414062</v>
+      </c>
+      <c r="F115" t="n">
+        <v>501710</v>
+      </c>
+      <c r="G115" t="n">
+        <v>3502280</v>
+      </c>
+      <c r="H115" t="n">
+        <v>4895.56005859375</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B116" t="n">
+        <v>5358</v>
+      </c>
+      <c r="C116" t="n">
+        <v>506709.4375</v>
+      </c>
+      <c r="D116" t="n">
+        <v>3505280.25</v>
+      </c>
+      <c r="E116" t="n">
+        <v>171.8500061035156</v>
+      </c>
+      <c r="F116" t="n">
+        <v>506710</v>
+      </c>
+      <c r="G116" t="n">
+        <v>3505280</v>
+      </c>
+      <c r="H116" t="n">
+        <v>5186.14990234375</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B117" t="n">
+        <v>5059</v>
+      </c>
+      <c r="C117" t="n">
+        <v>501740.125</v>
+      </c>
+      <c r="D117" t="n">
+        <v>3502320</v>
+      </c>
+      <c r="E117" t="n">
+        <v>162.3300018310547</v>
+      </c>
+      <c r="F117" t="n">
+        <v>501740</v>
+      </c>
+      <c r="G117" t="n">
+        <v>3502320</v>
+      </c>
+      <c r="H117" t="n">
+        <v>4896.669921875</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B118" t="n">
+        <v>5359</v>
+      </c>
+      <c r="C118" t="n">
+        <v>506740.4375</v>
+      </c>
+      <c r="D118" t="n">
+        <v>3505320.75</v>
+      </c>
+      <c r="E118" t="n">
+        <v>172.2599945068359</v>
+      </c>
+      <c r="F118" t="n">
+        <v>506740</v>
+      </c>
+      <c r="G118" t="n">
+        <v>3505320</v>
+      </c>
+      <c r="H118" t="n">
+        <v>5186.740234375</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B119" t="n">
+        <v>5060</v>
+      </c>
+      <c r="C119" t="n">
+        <v>501770.4375</v>
+      </c>
+      <c r="D119" t="n">
+        <v>3502360</v>
+      </c>
+      <c r="E119" t="n">
+        <v>162.8600006103516</v>
+      </c>
+      <c r="F119" t="n">
+        <v>501770</v>
+      </c>
+      <c r="G119" t="n">
+        <v>3502360</v>
+      </c>
+      <c r="H119" t="n">
+        <v>4897.14013671875</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B120" t="n">
         <v>5360</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C120" t="n">
         <v>506769.4375</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D120" t="n">
         <v>3505360.75</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E120" t="n">
         <v>172.0500030517578</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F120" t="n">
         <v>506770</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G120" t="n">
         <v>3505360</v>
       </c>
-      <c r="G3" t="n">
-        <v>172.3899993896484</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1.031794548034668</v>
+      <c r="H120" t="n">
+        <v>5187.9501953125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move optional input for graph to Google Drive or local options when writing the data in files, add warning message if data have been written more than once.
</commit_message>
<xml_diff>
--- a/qcdata/QCSDA.xlsx
+++ b/qcdata/QCSDA.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -562,6 +562,202 @@
         <v>135</v>
       </c>
       <c r="D8" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B9" t="n">
+        <v>120</v>
+      </c>
+      <c r="C9" t="n">
+        <v>135</v>
+      </c>
+      <c r="D9" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B10" t="n">
+        <v>120</v>
+      </c>
+      <c r="C10" t="n">
+        <v>135</v>
+      </c>
+      <c r="D10" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B11" t="n">
+        <v>120</v>
+      </c>
+      <c r="C11" t="n">
+        <v>135</v>
+      </c>
+      <c r="D11" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B12" t="n">
+        <v>120</v>
+      </c>
+      <c r="C12" t="n">
+        <v>135</v>
+      </c>
+      <c r="D12" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B13" t="n">
+        <v>120</v>
+      </c>
+      <c r="C13" t="n">
+        <v>135</v>
+      </c>
+      <c r="D13" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B14" t="n">
+        <v>120</v>
+      </c>
+      <c r="C14" t="n">
+        <v>135</v>
+      </c>
+      <c r="D14" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B15" t="n">
+        <v>120</v>
+      </c>
+      <c r="C15" t="n">
+        <v>135</v>
+      </c>
+      <c r="D15" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B16" t="n">
+        <v>120</v>
+      </c>
+      <c r="C16" t="n">
+        <v>135</v>
+      </c>
+      <c r="D16" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B17" t="n">
+        <v>120</v>
+      </c>
+      <c r="C17" t="n">
+        <v>135</v>
+      </c>
+      <c r="D17" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B18" t="n">
+        <v>120</v>
+      </c>
+      <c r="C18" t="n">
+        <v>135</v>
+      </c>
+      <c r="D18" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B19" t="n">
+        <v>120</v>
+      </c>
+      <c r="C19" t="n">
+        <v>135</v>
+      </c>
+      <c r="D19" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B20" t="n">
+        <v>120</v>
+      </c>
+      <c r="C20" t="n">
+        <v>135</v>
+      </c>
+      <c r="D20" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B21" t="n">
+        <v>120</v>
+      </c>
+      <c r="C21" t="n">
+        <v>135</v>
+      </c>
+      <c r="D21" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B22" t="n">
+        <v>120</v>
+      </c>
+      <c r="C22" t="n">
+        <v>135</v>
+      </c>
+      <c r="D22" t="n">
         <v>119</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correct formula to obtain points out of specifications by positioning issues and improve some visualization lines
</commit_message>
<xml_diff>
--- a/qcdata/QCSDA.xlsx
+++ b/qcdata/QCSDA.xlsx
@@ -8,9 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Redo_distortion_2021-08-10" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Redo_force_2021-08-10" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Redo_COG_2021-08-10" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Redo_distortion_10-08-2021" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Redo_force_10-08-2021" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Redo_COG_10-08-2021" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -772,6 +772,36 @@
         <v>135</v>
       </c>
       <c r="D23" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n">
+        <v>44418</v>
+      </c>
+      <c r="B24" t="n">
+        <v>120</v>
+      </c>
+      <c r="C24" t="n">
+        <v>135</v>
+      </c>
+      <c r="D24" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10-08-2021</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>120</v>
+      </c>
+      <c r="C25" t="n">
+        <v>135</v>
+      </c>
+      <c r="D25" t="n">
         <v>119</v>
       </c>
     </row>
@@ -2001,7 +2031,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H136"/>
+  <dimension ref="A1:H134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2014,7 +2044,7 @@
         <v>1001</v>
       </c>
       <c r="B1" t="n">
-        <v>5001</v>
+        <v>5002</v>
       </c>
       <c r="C1" t="n">
         <v>1</v>
@@ -2023,16 +2053,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="n">
-        <v>68.77999877929688</v>
+        <v>80.08999633789062</v>
       </c>
       <c r="F1" t="n">
-        <v>500000</v>
+        <v>500030</v>
       </c>
       <c r="G1" t="n">
-        <v>3500000</v>
+        <v>3500030</v>
       </c>
       <c r="H1" t="n">
-        <v>150</v>
+        <v>150.2100067138672</v>
       </c>
     </row>
     <row r="2">
@@ -2040,25 +2070,25 @@
         <v>1001</v>
       </c>
       <c r="B2" t="n">
-        <v>5001</v>
+        <v>5302</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>68.79000091552734</v>
+        <v>80.70999908447266</v>
       </c>
       <c r="F2" t="n">
-        <v>500000</v>
+        <v>505030</v>
       </c>
       <c r="G2" t="n">
-        <v>3500000</v>
+        <v>3503030</v>
       </c>
       <c r="H2" t="n">
-        <v>150</v>
+        <v>160.2100067138672</v>
       </c>
     </row>
     <row r="3">
@@ -2066,25 +2096,25 @@
         <v>1001</v>
       </c>
       <c r="B3" t="n">
-        <v>5301</v>
+        <v>5303</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>68.26999664306641</v>
+        <v>80.83999633789062</v>
       </c>
       <c r="F3" t="n">
-        <v>505000</v>
+        <v>505060</v>
       </c>
       <c r="G3" t="n">
-        <v>3503000</v>
+        <v>3503060</v>
       </c>
       <c r="H3" t="n">
-        <v>160</v>
+        <v>160.4199981689453</v>
       </c>
     </row>
     <row r="4">
@@ -2092,25 +2122,25 @@
         <v>1001</v>
       </c>
       <c r="B4" t="n">
-        <v>5002</v>
+        <v>5303</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>69.37000274658203</v>
+        <v>81.81999969482422</v>
       </c>
       <c r="F4" t="n">
-        <v>500030</v>
+        <v>505060</v>
       </c>
       <c r="G4" t="n">
-        <v>3500030</v>
+        <v>3503060</v>
       </c>
       <c r="H4" t="n">
-        <v>150.2100067138672</v>
+        <v>160.4199981689453</v>
       </c>
     </row>
     <row r="5">
@@ -2118,25 +2148,25 @@
         <v>1001</v>
       </c>
       <c r="B5" t="n">
-        <v>5302</v>
+        <v>5005</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>69.51000213623047</v>
+        <v>81.13999938964844</v>
       </c>
       <c r="F5" t="n">
-        <v>505030</v>
+        <v>500120</v>
       </c>
       <c r="G5" t="n">
-        <v>3503030</v>
+        <v>3500120</v>
       </c>
       <c r="H5" t="n">
-        <v>160.2100067138672</v>
+        <v>150.8399963378906</v>
       </c>
     </row>
     <row r="6">
@@ -2144,25 +2174,25 @@
         <v>1001</v>
       </c>
       <c r="B6" t="n">
-        <v>5003</v>
+        <v>5005</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>68.05999755859375</v>
+        <v>81.19000244140625</v>
       </c>
       <c r="F6" t="n">
-        <v>500060</v>
+        <v>500120</v>
       </c>
       <c r="G6" t="n">
-        <v>3500060</v>
+        <v>3500120</v>
       </c>
       <c r="H6" t="n">
-        <v>150.4199981689453</v>
+        <v>150.8399963378906</v>
       </c>
     </row>
     <row r="7">
@@ -2170,25 +2200,25 @@
         <v>1001</v>
       </c>
       <c r="B7" t="n">
-        <v>5004</v>
+        <v>5306</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>69.41000366210938</v>
+        <v>80.13999938964844</v>
       </c>
       <c r="F7" t="n">
-        <v>500090</v>
+        <v>505150</v>
       </c>
       <c r="G7" t="n">
-        <v>3500090</v>
+        <v>3503150</v>
       </c>
       <c r="H7" t="n">
-        <v>150.6300048828125</v>
+        <v>161.0500030517578</v>
       </c>
     </row>
     <row r="8">
@@ -2196,25 +2226,25 @@
         <v>1001</v>
       </c>
       <c r="B8" t="n">
-        <v>5304</v>
+        <v>5310</v>
       </c>
       <c r="C8" t="n">
         <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>69.16000366210938</v>
+        <v>80.61000061035156</v>
       </c>
       <c r="F8" t="n">
-        <v>505090</v>
+        <v>505270</v>
       </c>
       <c r="G8" t="n">
-        <v>3503090</v>
+        <v>3503270</v>
       </c>
       <c r="H8" t="n">
-        <v>160.6300048828125</v>
+        <v>161.8899993896484</v>
       </c>
     </row>
     <row r="9">
@@ -2222,7 +2252,7 @@
         <v>1001</v>
       </c>
       <c r="B9" t="n">
-        <v>5306</v>
+        <v>5310</v>
       </c>
       <c r="C9" t="n">
         <v>2</v>
@@ -2231,16 +2261,16 @@
         <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>69.58000183105469</v>
+        <v>81.15000152587891</v>
       </c>
       <c r="F9" t="n">
-        <v>505150</v>
+        <v>505270</v>
       </c>
       <c r="G9" t="n">
-        <v>3503150</v>
+        <v>3503270</v>
       </c>
       <c r="H9" t="n">
-        <v>161.0500030517578</v>
+        <v>161.8899993896484</v>
       </c>
     </row>
     <row r="10">
@@ -2248,25 +2278,25 @@
         <v>1001</v>
       </c>
       <c r="B10" t="n">
-        <v>5307</v>
+        <v>5012</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>69.95999908447266</v>
+        <v>81.37000274658203</v>
       </c>
       <c r="F10" t="n">
-        <v>505180</v>
+        <v>500330</v>
       </c>
       <c r="G10" t="n">
-        <v>3503180</v>
+        <v>3500330</v>
       </c>
       <c r="H10" t="n">
-        <v>161.2599945068359</v>
+        <v>152.3099975585938</v>
       </c>
     </row>
     <row r="11">
@@ -2274,25 +2304,25 @@
         <v>1001</v>
       </c>
       <c r="B11" t="n">
-        <v>5008</v>
+        <v>5012</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11" t="n">
-        <v>69.22000122070312</v>
+        <v>81.45999908447266</v>
       </c>
       <c r="F11" t="n">
-        <v>500210</v>
+        <v>500330</v>
       </c>
       <c r="G11" t="n">
-        <v>3500210</v>
+        <v>3500330</v>
       </c>
       <c r="H11" t="n">
-        <v>151.4700012207031</v>
+        <v>152.3099975585938</v>
       </c>
     </row>
     <row r="12">
@@ -2300,7 +2330,7 @@
         <v>1001</v>
       </c>
       <c r="B12" t="n">
-        <v>5308</v>
+        <v>5313</v>
       </c>
       <c r="C12" t="n">
         <v>2</v>
@@ -2309,16 +2339,16 @@
         <v>7</v>
       </c>
       <c r="E12" t="n">
-        <v>69.66999816894531</v>
+        <v>80.47000122070312</v>
       </c>
       <c r="F12" t="n">
-        <v>505210</v>
+        <v>505360</v>
       </c>
       <c r="G12" t="n">
-        <v>3503210</v>
+        <v>3503360</v>
       </c>
       <c r="H12" t="n">
-        <v>161.4700012207031</v>
+        <v>162.5200042724609</v>
       </c>
     </row>
     <row r="13">
@@ -2326,7 +2356,7 @@
         <v>1001</v>
       </c>
       <c r="B13" t="n">
-        <v>5009</v>
+        <v>5014</v>
       </c>
       <c r="C13" t="n">
         <v>1</v>
@@ -2335,16 +2365,16 @@
         <v>4</v>
       </c>
       <c r="E13" t="n">
-        <v>69.04000091552734</v>
+        <v>80.73999786376953</v>
       </c>
       <c r="F13" t="n">
-        <v>500240</v>
+        <v>500390</v>
       </c>
       <c r="G13" t="n">
-        <v>3500240</v>
+        <v>3500390</v>
       </c>
       <c r="H13" t="n">
-        <v>151.6799926757812</v>
+        <v>152.7299957275391</v>
       </c>
     </row>
     <row r="14">
@@ -2352,25 +2382,25 @@
         <v>1001</v>
       </c>
       <c r="B14" t="n">
-        <v>5309</v>
+        <v>5314</v>
       </c>
       <c r="C14" t="n">
         <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" t="n">
-        <v>68.05000305175781</v>
+        <v>80.73000335693359</v>
       </c>
       <c r="F14" t="n">
-        <v>505240</v>
+        <v>505390</v>
       </c>
       <c r="G14" t="n">
-        <v>3503240</v>
+        <v>3503390</v>
       </c>
       <c r="H14" t="n">
-        <v>161.6799926757812</v>
+        <v>162.7299957275391</v>
       </c>
     </row>
     <row r="15">
@@ -2378,25 +2408,25 @@
         <v>1001</v>
       </c>
       <c r="B15" t="n">
-        <v>5309</v>
+        <v>5015</v>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E15" t="n">
-        <v>68.01999664306641</v>
+        <v>80.66000366210938</v>
       </c>
       <c r="F15" t="n">
-        <v>505240</v>
+        <v>500420</v>
       </c>
       <c r="G15" t="n">
-        <v>3503240</v>
+        <v>3500420</v>
       </c>
       <c r="H15" t="n">
-        <v>161.6799926757812</v>
+        <v>152.9400024414062</v>
       </c>
     </row>
     <row r="16">
@@ -2404,7 +2434,7 @@
         <v>1001</v>
       </c>
       <c r="B16" t="n">
-        <v>5010</v>
+        <v>5017</v>
       </c>
       <c r="C16" t="n">
         <v>1</v>
@@ -2413,16 +2443,16 @@
         <v>2</v>
       </c>
       <c r="E16" t="n">
-        <v>69.98999786376953</v>
+        <v>81.38999938964844</v>
       </c>
       <c r="F16" t="n">
-        <v>500270</v>
+        <v>500480</v>
       </c>
       <c r="G16" t="n">
-        <v>3500270</v>
+        <v>3500480</v>
       </c>
       <c r="H16" t="n">
-        <v>151.8899993896484</v>
+        <v>153.3600006103516</v>
       </c>
     </row>
     <row r="17">
@@ -2430,25 +2460,25 @@
         <v>1001</v>
       </c>
       <c r="B17" t="n">
-        <v>5310</v>
+        <v>5017</v>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E17" t="n">
-        <v>69.94000244140625</v>
+        <v>81.09999847412109</v>
       </c>
       <c r="F17" t="n">
-        <v>505270</v>
+        <v>500480</v>
       </c>
       <c r="G17" t="n">
-        <v>3503270</v>
+        <v>3500480</v>
       </c>
       <c r="H17" t="n">
-        <v>161.8899993896484</v>
+        <v>153.3600006103516</v>
       </c>
     </row>
     <row r="18">
@@ -2456,25 +2486,25 @@
         <v>1001</v>
       </c>
       <c r="B18" t="n">
-        <v>5311</v>
+        <v>5021</v>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E18" t="n">
-        <v>68.95999908447266</v>
+        <v>81.25</v>
       </c>
       <c r="F18" t="n">
-        <v>505300</v>
+        <v>500600</v>
       </c>
       <c r="G18" t="n">
-        <v>3503300</v>
+        <v>3500600</v>
       </c>
       <c r="H18" t="n">
-        <v>162.1000061035156</v>
+        <v>154.1999969482422</v>
       </c>
     </row>
     <row r="19">
@@ -2482,25 +2512,25 @@
         <v>1001</v>
       </c>
       <c r="B19" t="n">
-        <v>5012</v>
+        <v>5021</v>
       </c>
       <c r="C19" t="n">
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E19" t="n">
-        <v>68.37000274658203</v>
+        <v>80.69000244140625</v>
       </c>
       <c r="F19" t="n">
-        <v>500330</v>
+        <v>500600</v>
       </c>
       <c r="G19" t="n">
-        <v>3500330</v>
+        <v>3500600</v>
       </c>
       <c r="H19" t="n">
-        <v>152.3099975585938</v>
+        <v>154.1999969482422</v>
       </c>
     </row>
     <row r="20">
@@ -2508,25 +2538,25 @@
         <v>1001</v>
       </c>
       <c r="B20" t="n">
-        <v>5312</v>
+        <v>5022</v>
       </c>
       <c r="C20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>68.09999847412109</v>
+        <v>81.59999847412109</v>
       </c>
       <c r="F20" t="n">
-        <v>505330</v>
+        <v>500630</v>
       </c>
       <c r="G20" t="n">
-        <v>3503330</v>
+        <v>3500630</v>
       </c>
       <c r="H20" t="n">
-        <v>162.3099975585938</v>
+        <v>154.4100036621094</v>
       </c>
     </row>
     <row r="21">
@@ -2534,25 +2564,25 @@
         <v>1001</v>
       </c>
       <c r="B21" t="n">
-        <v>5015</v>
+        <v>5323</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E21" t="n">
-        <v>68.45999908447266</v>
+        <v>81.72000122070312</v>
       </c>
       <c r="F21" t="n">
-        <v>500420</v>
+        <v>505660</v>
       </c>
       <c r="G21" t="n">
-        <v>3500420</v>
+        <v>3503660</v>
       </c>
       <c r="H21" t="n">
-        <v>152.9400024414062</v>
+        <v>164.6199951171875</v>
       </c>
     </row>
     <row r="22">
@@ -2560,25 +2590,25 @@
         <v>1001</v>
       </c>
       <c r="B22" t="n">
-        <v>5016</v>
+        <v>5323</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E22" t="n">
-        <v>68.68000030517578</v>
+        <v>81.47000122070312</v>
       </c>
       <c r="F22" t="n">
-        <v>500450</v>
+        <v>505660</v>
       </c>
       <c r="G22" t="n">
-        <v>3500450</v>
+        <v>3503660</v>
       </c>
       <c r="H22" t="n">
-        <v>153.1499938964844</v>
+        <v>164.6199951171875</v>
       </c>
     </row>
     <row r="23">
@@ -2586,25 +2616,25 @@
         <v>1001</v>
       </c>
       <c r="B23" t="n">
-        <v>5018</v>
+        <v>5024</v>
       </c>
       <c r="C23" t="n">
         <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E23" t="n">
-        <v>68.01999664306641</v>
+        <v>81.05999755859375</v>
       </c>
       <c r="F23" t="n">
-        <v>500510</v>
+        <v>500690</v>
       </c>
       <c r="G23" t="n">
-        <v>3500510</v>
+        <v>3500690</v>
       </c>
       <c r="H23" t="n">
-        <v>153.5700073242188</v>
+        <v>154.8300018310547</v>
       </c>
     </row>
     <row r="24">
@@ -2612,25 +2642,25 @@
         <v>1001</v>
       </c>
       <c r="B24" t="n">
-        <v>5319</v>
+        <v>5027</v>
       </c>
       <c r="C24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>69.73000335693359</v>
+        <v>81.59999847412109</v>
       </c>
       <c r="F24" t="n">
-        <v>505540</v>
+        <v>500780</v>
       </c>
       <c r="G24" t="n">
-        <v>3503540</v>
+        <v>3500780</v>
       </c>
       <c r="H24" t="n">
-        <v>163.7799987792969</v>
+        <v>155.4600067138672</v>
       </c>
     </row>
     <row r="25">
@@ -2638,25 +2668,25 @@
         <v>1001</v>
       </c>
       <c r="B25" t="n">
-        <v>5020</v>
+        <v>5327</v>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E25" t="n">
-        <v>69.29000091552734</v>
+        <v>81.40000152587891</v>
       </c>
       <c r="F25" t="n">
-        <v>500570</v>
+        <v>505780</v>
       </c>
       <c r="G25" t="n">
-        <v>3500570</v>
+        <v>3503780</v>
       </c>
       <c r="H25" t="n">
-        <v>153.9900054931641</v>
+        <v>165.4600067138672</v>
       </c>
     </row>
     <row r="26">
@@ -2664,25 +2694,25 @@
         <v>1001</v>
       </c>
       <c r="B26" t="n">
-        <v>5320</v>
+        <v>5328</v>
       </c>
       <c r="C26" t="n">
         <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E26" t="n">
-        <v>68.13999938964844</v>
+        <v>80.01999664306641</v>
       </c>
       <c r="F26" t="n">
-        <v>505570</v>
+        <v>505810</v>
       </c>
       <c r="G26" t="n">
-        <v>3503570</v>
+        <v>3503810</v>
       </c>
       <c r="H26" t="n">
-        <v>163.9900054931641</v>
+        <v>165.6699981689453</v>
       </c>
     </row>
     <row r="27">
@@ -2690,7 +2720,7 @@
         <v>1001</v>
       </c>
       <c r="B27" t="n">
-        <v>5321</v>
+        <v>5328</v>
       </c>
       <c r="C27" t="n">
         <v>2</v>
@@ -2699,16 +2729,16 @@
         <v>6</v>
       </c>
       <c r="E27" t="n">
-        <v>68.34999847412109</v>
+        <v>80.75</v>
       </c>
       <c r="F27" t="n">
-        <v>505600</v>
+        <v>505810</v>
       </c>
       <c r="G27" t="n">
-        <v>3503600</v>
+        <v>3503810</v>
       </c>
       <c r="H27" t="n">
-        <v>164.1999969482422</v>
+        <v>165.6699981689453</v>
       </c>
     </row>
     <row r="28">
@@ -2716,25 +2746,25 @@
         <v>1001</v>
       </c>
       <c r="B28" t="n">
-        <v>5022</v>
+        <v>5329</v>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E28" t="n">
-        <v>68.80000305175781</v>
+        <v>81.83999633789062</v>
       </c>
       <c r="F28" t="n">
-        <v>500630</v>
+        <v>505840</v>
       </c>
       <c r="G28" t="n">
-        <v>3500630</v>
+        <v>3503840</v>
       </c>
       <c r="H28" t="n">
-        <v>154.4100036621094</v>
+        <v>165.8800048828125</v>
       </c>
     </row>
     <row r="29">
@@ -2742,25 +2772,25 @@
         <v>1001</v>
       </c>
       <c r="B29" t="n">
-        <v>5023</v>
+        <v>5330</v>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E29" t="n">
-        <v>69.62999725341797</v>
+        <v>80.01999664306641</v>
       </c>
       <c r="F29" t="n">
-        <v>500660</v>
+        <v>505870</v>
       </c>
       <c r="G29" t="n">
-        <v>3500660</v>
+        <v>3503870</v>
       </c>
       <c r="H29" t="n">
-        <v>154.6199951171875</v>
+        <v>166.0899963378906</v>
       </c>
     </row>
     <row r="30">
@@ -2768,25 +2798,25 @@
         <v>1001</v>
       </c>
       <c r="B30" t="n">
-        <v>5023</v>
+        <v>5331</v>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E30" t="n">
-        <v>68.80999755859375</v>
+        <v>81.62000274658203</v>
       </c>
       <c r="F30" t="n">
-        <v>500660</v>
+        <v>505900</v>
       </c>
       <c r="G30" t="n">
-        <v>3500660</v>
+        <v>3503900</v>
       </c>
       <c r="H30" t="n">
-        <v>154.6199951171875</v>
+        <v>166.3000030517578</v>
       </c>
     </row>
     <row r="31">
@@ -2794,25 +2824,25 @@
         <v>1001</v>
       </c>
       <c r="B31" t="n">
-        <v>5025</v>
+        <v>5032</v>
       </c>
       <c r="C31" t="n">
         <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E31" t="n">
-        <v>69.83999633789062</v>
+        <v>80.76000213623047</v>
       </c>
       <c r="F31" t="n">
-        <v>500720</v>
+        <v>500930</v>
       </c>
       <c r="G31" t="n">
-        <v>3500720</v>
+        <v>3500930</v>
       </c>
       <c r="H31" t="n">
-        <v>155.0399932861328</v>
+        <v>156.5099945068359</v>
       </c>
     </row>
     <row r="32">
@@ -2820,25 +2850,25 @@
         <v>1001</v>
       </c>
       <c r="B32" t="n">
-        <v>5025</v>
+        <v>5033</v>
       </c>
       <c r="C32" t="n">
         <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E32" t="n">
-        <v>69.27999877929688</v>
+        <v>81.26999664306641</v>
       </c>
       <c r="F32" t="n">
-        <v>500720</v>
+        <v>500960</v>
       </c>
       <c r="G32" t="n">
-        <v>3500720</v>
+        <v>3500960</v>
       </c>
       <c r="H32" t="n">
-        <v>155.0399932861328</v>
+        <v>156.7200012207031</v>
       </c>
     </row>
     <row r="33">
@@ -2846,25 +2876,25 @@
         <v>1001</v>
       </c>
       <c r="B33" t="n">
-        <v>5325</v>
+        <v>5035</v>
       </c>
       <c r="C33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E33" t="n">
-        <v>68.15000152587891</v>
+        <v>80.70999908447266</v>
       </c>
       <c r="F33" t="n">
-        <v>505720</v>
+        <v>501020</v>
       </c>
       <c r="G33" t="n">
-        <v>3503720</v>
+        <v>3501020</v>
       </c>
       <c r="H33" t="n">
-        <v>165.0399932861328</v>
+        <v>157.1399993896484</v>
       </c>
     </row>
     <row r="34">
@@ -2872,25 +2902,25 @@
         <v>1001</v>
       </c>
       <c r="B34" t="n">
-        <v>5026</v>
+        <v>5336</v>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E34" t="n">
-        <v>68.86000061035156</v>
+        <v>80.19999694824219</v>
       </c>
       <c r="F34" t="n">
-        <v>500750</v>
+        <v>506050</v>
       </c>
       <c r="G34" t="n">
-        <v>3500750</v>
+        <v>3504050</v>
       </c>
       <c r="H34" t="n">
-        <v>155.25</v>
+        <v>167.3500061035156</v>
       </c>
     </row>
     <row r="35">
@@ -2898,25 +2928,25 @@
         <v>1001</v>
       </c>
       <c r="B35" t="n">
-        <v>5028</v>
+        <v>5037</v>
       </c>
       <c r="C35" t="n">
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E35" t="n">
-        <v>69.26000213623047</v>
+        <v>81.65000152587891</v>
       </c>
       <c r="F35" t="n">
-        <v>500810</v>
+        <v>501080</v>
       </c>
       <c r="G35" t="n">
-        <v>3500810</v>
+        <v>3501080</v>
       </c>
       <c r="H35" t="n">
-        <v>155.6699981689453</v>
+        <v>157.5599975585938</v>
       </c>
     </row>
     <row r="36">
@@ -2924,25 +2954,25 @@
         <v>1001</v>
       </c>
       <c r="B36" t="n">
-        <v>5329</v>
+        <v>5038</v>
       </c>
       <c r="C36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E36" t="n">
-        <v>69.26000213623047</v>
+        <v>81.93000030517578</v>
       </c>
       <c r="F36" t="n">
-        <v>505840</v>
+        <v>501110</v>
       </c>
       <c r="G36" t="n">
-        <v>3503840</v>
+        <v>3501110</v>
       </c>
       <c r="H36" t="n">
-        <v>165.8800048828125</v>
+        <v>157.7700042724609</v>
       </c>
     </row>
     <row r="37">
@@ -2950,25 +2980,25 @@
         <v>1001</v>
       </c>
       <c r="B37" t="n">
-        <v>5030</v>
+        <v>5338</v>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E37" t="n">
-        <v>68.84999847412109</v>
+        <v>81.88999938964844</v>
       </c>
       <c r="F37" t="n">
-        <v>500870</v>
+        <v>506110</v>
       </c>
       <c r="G37" t="n">
-        <v>3500870</v>
+        <v>3504110</v>
       </c>
       <c r="H37" t="n">
-        <v>156.0899963378906</v>
+        <v>167.7700042724609</v>
       </c>
     </row>
     <row r="38">
@@ -2976,25 +3006,25 @@
         <v>1001</v>
       </c>
       <c r="B38" t="n">
-        <v>5031</v>
+        <v>5339</v>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E38" t="n">
-        <v>69.54000091552734</v>
+        <v>80.73999786376953</v>
       </c>
       <c r="F38" t="n">
-        <v>500900</v>
+        <v>506140</v>
       </c>
       <c r="G38" t="n">
-        <v>3500900</v>
+        <v>3504140</v>
       </c>
       <c r="H38" t="n">
-        <v>156.3000030517578</v>
+        <v>167.9799957275391</v>
       </c>
     </row>
     <row r="39">
@@ -3002,25 +3032,25 @@
         <v>1001</v>
       </c>
       <c r="B39" t="n">
-        <v>5031</v>
+        <v>5040</v>
       </c>
       <c r="C39" t="n">
         <v>1</v>
       </c>
       <c r="D39" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E39" t="n">
-        <v>69.54000091552734</v>
+        <v>81.25</v>
       </c>
       <c r="F39" t="n">
-        <v>500900</v>
+        <v>501170</v>
       </c>
       <c r="G39" t="n">
-        <v>3500900</v>
+        <v>3501170</v>
       </c>
       <c r="H39" t="n">
-        <v>156.3000030517578</v>
+        <v>158.1900024414062</v>
       </c>
     </row>
     <row r="40">
@@ -3028,25 +3058,25 @@
         <v>1001</v>
       </c>
       <c r="B40" t="n">
-        <v>5332</v>
+        <v>5041</v>
       </c>
       <c r="C40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E40" t="n">
-        <v>69.23999786376953</v>
+        <v>81.91999816894531</v>
       </c>
       <c r="F40" t="n">
-        <v>505930</v>
+        <v>501200</v>
       </c>
       <c r="G40" t="n">
-        <v>3503930</v>
+        <v>3501200</v>
       </c>
       <c r="H40" t="n">
-        <v>166.5099945068359</v>
+        <v>158.3999938964844</v>
       </c>
     </row>
     <row r="41">
@@ -3054,7 +3084,7 @@
         <v>1001</v>
       </c>
       <c r="B41" t="n">
-        <v>5033</v>
+        <v>5041</v>
       </c>
       <c r="C41" t="n">
         <v>1</v>
@@ -3063,16 +3093,16 @@
         <v>3</v>
       </c>
       <c r="E41" t="n">
-        <v>68.84999847412109</v>
+        <v>81.47000122070312</v>
       </c>
       <c r="F41" t="n">
-        <v>500960</v>
+        <v>501200</v>
       </c>
       <c r="G41" t="n">
-        <v>3500960</v>
+        <v>3501200</v>
       </c>
       <c r="H41" t="n">
-        <v>156.7200012207031</v>
+        <v>158.3999938964844</v>
       </c>
     </row>
     <row r="42">
@@ -3080,7 +3110,7 @@
         <v>1001</v>
       </c>
       <c r="B42" t="n">
-        <v>5334</v>
+        <v>5341</v>
       </c>
       <c r="C42" t="n">
         <v>2</v>
@@ -3089,16 +3119,16 @@
         <v>6</v>
       </c>
       <c r="E42" t="n">
-        <v>69.87000274658203</v>
+        <v>81.08999633789062</v>
       </c>
       <c r="F42" t="n">
-        <v>505990</v>
+        <v>506200</v>
       </c>
       <c r="G42" t="n">
-        <v>3503990</v>
+        <v>3504200</v>
       </c>
       <c r="H42" t="n">
-        <v>166.9299926757812</v>
+        <v>168.3999938964844</v>
       </c>
     </row>
     <row r="43">
@@ -3106,25 +3136,25 @@
         <v>1001</v>
       </c>
       <c r="B43" t="n">
-        <v>5335</v>
+        <v>5342</v>
       </c>
       <c r="C43" t="n">
         <v>2</v>
       </c>
       <c r="D43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E43" t="n">
-        <v>68.45999908447266</v>
+        <v>81.94000244140625</v>
       </c>
       <c r="F43" t="n">
-        <v>506020</v>
+        <v>506230</v>
       </c>
       <c r="G43" t="n">
-        <v>3504020</v>
+        <v>3504230</v>
       </c>
       <c r="H43" t="n">
-        <v>167.1399993896484</v>
+        <v>168.6100006103516</v>
       </c>
     </row>
     <row r="44">
@@ -3132,25 +3162,25 @@
         <v>1001</v>
       </c>
       <c r="B44" t="n">
-        <v>5335</v>
+        <v>5342</v>
       </c>
       <c r="C44" t="n">
         <v>2</v>
       </c>
       <c r="D44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E44" t="n">
-        <v>68.75</v>
+        <v>81.47000122070312</v>
       </c>
       <c r="F44" t="n">
-        <v>506020</v>
+        <v>506230</v>
       </c>
       <c r="G44" t="n">
-        <v>3504020</v>
+        <v>3504230</v>
       </c>
       <c r="H44" t="n">
-        <v>167.1399993896484</v>
+        <v>168.6100006103516</v>
       </c>
     </row>
     <row r="45">
@@ -3158,25 +3188,25 @@
         <v>1001</v>
       </c>
       <c r="B45" t="n">
-        <v>5037</v>
+        <v>5342</v>
       </c>
       <c r="C45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E45" t="n">
-        <v>69.05999755859375</v>
+        <v>81.48999786376953</v>
       </c>
       <c r="F45" t="n">
-        <v>501080</v>
+        <v>506230</v>
       </c>
       <c r="G45" t="n">
-        <v>3501080</v>
+        <v>3504230</v>
       </c>
       <c r="H45" t="n">
-        <v>157.5599975585938</v>
+        <v>168.6100006103516</v>
       </c>
     </row>
     <row r="46">
@@ -3184,25 +3214,25 @@
         <v>1001</v>
       </c>
       <c r="B46" t="n">
-        <v>5039</v>
+        <v>5343</v>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E46" t="n">
-        <v>69.02999877929688</v>
+        <v>80.62000274658203</v>
       </c>
       <c r="F46" t="n">
-        <v>501140</v>
+        <v>506260</v>
       </c>
       <c r="G46" t="n">
-        <v>3501140</v>
+        <v>3504260</v>
       </c>
       <c r="H46" t="n">
-        <v>157.9799957275391</v>
+        <v>168.8200073242188</v>
       </c>
     </row>
     <row r="47">
@@ -3210,25 +3240,25 @@
         <v>1001</v>
       </c>
       <c r="B47" t="n">
-        <v>5040</v>
+        <v>5345</v>
       </c>
       <c r="C47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E47" t="n">
-        <v>68.55000305175781</v>
+        <v>80.31999969482422</v>
       </c>
       <c r="F47" t="n">
-        <v>501170</v>
+        <v>506320</v>
       </c>
       <c r="G47" t="n">
-        <v>3501170</v>
+        <v>3504320</v>
       </c>
       <c r="H47" t="n">
-        <v>158.1900024414062</v>
+        <v>169.2400054931641</v>
       </c>
     </row>
     <row r="48">
@@ -3236,25 +3266,25 @@
         <v>1001</v>
       </c>
       <c r="B48" t="n">
-        <v>5043</v>
+        <v>5046</v>
       </c>
       <c r="C48" t="n">
         <v>1</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E48" t="n">
-        <v>69.62000274658203</v>
+        <v>81.55999755859375</v>
       </c>
       <c r="F48" t="n">
-        <v>501260</v>
+        <v>501350</v>
       </c>
       <c r="G48" t="n">
-        <v>3501260</v>
+        <v>3501350</v>
       </c>
       <c r="H48" t="n">
-        <v>158.8200073242188</v>
+        <v>159.4499969482422</v>
       </c>
     </row>
     <row r="49">
@@ -3262,25 +3292,25 @@
         <v>1001</v>
       </c>
       <c r="B49" t="n">
-        <v>5043</v>
+        <v>5346</v>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E49" t="n">
-        <v>68.72000122070312</v>
+        <v>80.27999877929688</v>
       </c>
       <c r="F49" t="n">
-        <v>501260</v>
+        <v>506350</v>
       </c>
       <c r="G49" t="n">
-        <v>3501260</v>
+        <v>3504350</v>
       </c>
       <c r="H49" t="n">
-        <v>158.8200073242188</v>
+        <v>169.4499969482422</v>
       </c>
     </row>
     <row r="50">
@@ -3288,25 +3318,25 @@
         <v>1001</v>
       </c>
       <c r="B50" t="n">
-        <v>5044</v>
+        <v>5047</v>
       </c>
       <c r="C50" t="n">
         <v>1</v>
       </c>
       <c r="D50" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E50" t="n">
-        <v>68.23000335693359</v>
+        <v>80.58000183105469</v>
       </c>
       <c r="F50" t="n">
-        <v>501290</v>
+        <v>501380</v>
       </c>
       <c r="G50" t="n">
-        <v>3501290</v>
+        <v>3501380</v>
       </c>
       <c r="H50" t="n">
-        <v>159.0299987792969</v>
+        <v>159.6600036621094</v>
       </c>
     </row>
     <row r="51">
@@ -3314,7 +3344,7 @@
         <v>1001</v>
       </c>
       <c r="B51" t="n">
-        <v>5348</v>
+        <v>5347</v>
       </c>
       <c r="C51" t="n">
         <v>2</v>
@@ -3323,16 +3353,16 @@
         <v>8</v>
       </c>
       <c r="E51" t="n">
-        <v>69</v>
+        <v>80.62999725341797</v>
       </c>
       <c r="F51" t="n">
-        <v>506410</v>
+        <v>506380</v>
       </c>
       <c r="G51" t="n">
-        <v>3504410</v>
+        <v>3504380</v>
       </c>
       <c r="H51" t="n">
-        <v>169.8699951171875</v>
+        <v>169.6600036621094</v>
       </c>
     </row>
     <row r="52">
@@ -3340,25 +3370,25 @@
         <v>1001</v>
       </c>
       <c r="B52" t="n">
-        <v>5049</v>
+        <v>5048</v>
       </c>
       <c r="C52" t="n">
         <v>1</v>
       </c>
       <c r="D52" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E52" t="n">
-        <v>69.30000305175781</v>
+        <v>81.36000061035156</v>
       </c>
       <c r="F52" t="n">
-        <v>501440</v>
+        <v>501410</v>
       </c>
       <c r="G52" t="n">
-        <v>3501440</v>
+        <v>3501410</v>
       </c>
       <c r="H52" t="n">
-        <v>160.0800018310547</v>
+        <v>159.8699951171875</v>
       </c>
     </row>
     <row r="53">
@@ -3366,25 +3396,25 @@
         <v>1001</v>
       </c>
       <c r="B53" t="n">
-        <v>5049</v>
+        <v>5349</v>
       </c>
       <c r="C53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D53" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E53" t="n">
-        <v>68.12999725341797</v>
+        <v>80.80999755859375</v>
       </c>
       <c r="F53" t="n">
-        <v>501440</v>
+        <v>506440</v>
       </c>
       <c r="G53" t="n">
-        <v>3501440</v>
+        <v>3504440</v>
       </c>
       <c r="H53" t="n">
-        <v>160.0800018310547</v>
+        <v>170.0800018310547</v>
       </c>
     </row>
     <row r="54">
@@ -3392,25 +3422,25 @@
         <v>1001</v>
       </c>
       <c r="B54" t="n">
-        <v>5349</v>
+        <v>5052</v>
       </c>
       <c r="C54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D54" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>68.01999664306641</v>
+        <v>81.48999786376953</v>
       </c>
       <c r="F54" t="n">
-        <v>506440</v>
+        <v>501530</v>
       </c>
       <c r="G54" t="n">
-        <v>3504440</v>
+        <v>3501530</v>
       </c>
       <c r="H54" t="n">
-        <v>170.0800018310547</v>
+        <v>160.7100067138672</v>
       </c>
     </row>
     <row r="55">
@@ -3418,25 +3448,25 @@
         <v>1001</v>
       </c>
       <c r="B55" t="n">
-        <v>5349</v>
+        <v>5053</v>
       </c>
       <c r="C55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D55" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E55" t="n">
-        <v>68.43000030517578</v>
+        <v>80.83999633789062</v>
       </c>
       <c r="F55" t="n">
-        <v>506440</v>
+        <v>501560</v>
       </c>
       <c r="G55" t="n">
-        <v>3504440</v>
+        <v>3501560</v>
       </c>
       <c r="H55" t="n">
-        <v>170.0800018310547</v>
+        <v>160.9199981689453</v>
       </c>
     </row>
     <row r="56">
@@ -3444,25 +3474,25 @@
         <v>1001</v>
       </c>
       <c r="B56" t="n">
-        <v>5050</v>
+        <v>5353</v>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E56" t="n">
-        <v>69.77999877929688</v>
+        <v>80.37999725341797</v>
       </c>
       <c r="F56" t="n">
-        <v>501470</v>
+        <v>506560</v>
       </c>
       <c r="G56" t="n">
-        <v>3501470</v>
+        <v>3504560</v>
       </c>
       <c r="H56" t="n">
-        <v>160.2899932861328</v>
+        <v>170.9199981689453</v>
       </c>
     </row>
     <row r="57">
@@ -3470,25 +3500,25 @@
         <v>1001</v>
       </c>
       <c r="B57" t="n">
-        <v>5050</v>
+        <v>5354</v>
       </c>
       <c r="C57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D57" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E57" t="n">
-        <v>68.12000274658203</v>
+        <v>81.98999786376953</v>
       </c>
       <c r="F57" t="n">
-        <v>501470</v>
+        <v>506590</v>
       </c>
       <c r="G57" t="n">
-        <v>3501470</v>
+        <v>3504590</v>
       </c>
       <c r="H57" t="n">
-        <v>160.2899932861328</v>
+        <v>171.1300048828125</v>
       </c>
     </row>
     <row r="58">
@@ -3496,25 +3526,25 @@
         <v>1001</v>
       </c>
       <c r="B58" t="n">
-        <v>5051</v>
+        <v>5354</v>
       </c>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D58" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E58" t="n">
-        <v>68.69000244140625</v>
+        <v>81.73000335693359</v>
       </c>
       <c r="F58" t="n">
-        <v>501500</v>
+        <v>506590</v>
       </c>
       <c r="G58" t="n">
-        <v>3501500</v>
+        <v>3504590</v>
       </c>
       <c r="H58" t="n">
-        <v>160.5</v>
+        <v>171.1300048828125</v>
       </c>
     </row>
     <row r="59">
@@ -3522,25 +3552,25 @@
         <v>1001</v>
       </c>
       <c r="B59" t="n">
-        <v>5051</v>
+        <v>5355</v>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D59" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E59" t="n">
-        <v>68.69000244140625</v>
+        <v>80.37999725341797</v>
       </c>
       <c r="F59" t="n">
-        <v>501500</v>
+        <v>506620</v>
       </c>
       <c r="G59" t="n">
-        <v>3501500</v>
+        <v>3504620</v>
       </c>
       <c r="H59" t="n">
-        <v>160.5</v>
+        <v>171.3399963378906</v>
       </c>
     </row>
     <row r="60">
@@ -3548,25 +3578,25 @@
         <v>1001</v>
       </c>
       <c r="B60" t="n">
-        <v>5051</v>
+        <v>5056</v>
       </c>
       <c r="C60" t="n">
         <v>1</v>
       </c>
       <c r="D60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E60" t="n">
-        <v>69.27999877929688</v>
+        <v>81.38999938964844</v>
       </c>
       <c r="F60" t="n">
-        <v>501500</v>
+        <v>501650</v>
       </c>
       <c r="G60" t="n">
-        <v>3501500</v>
+        <v>3501650</v>
       </c>
       <c r="H60" t="n">
-        <v>160.5</v>
+        <v>161.5500030517578</v>
       </c>
     </row>
     <row r="61">
@@ -3574,25 +3604,25 @@
         <v>1001</v>
       </c>
       <c r="B61" t="n">
-        <v>5354</v>
+        <v>5057</v>
       </c>
       <c r="C61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E61" t="n">
-        <v>69.77999877929688</v>
+        <v>81.70999908447266</v>
       </c>
       <c r="F61" t="n">
-        <v>506590</v>
+        <v>501680</v>
       </c>
       <c r="G61" t="n">
-        <v>3504590</v>
+        <v>3501680</v>
       </c>
       <c r="H61" t="n">
-        <v>171.1300048828125</v>
+        <v>161.7599945068359</v>
       </c>
     </row>
     <row r="62">
@@ -3600,25 +3630,25 @@
         <v>1001</v>
       </c>
       <c r="B62" t="n">
-        <v>5055</v>
+        <v>5357</v>
       </c>
       <c r="C62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D62" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E62" t="n">
-        <v>68.33000183105469</v>
+        <v>80.73000335693359</v>
       </c>
       <c r="F62" t="n">
-        <v>501620</v>
+        <v>506680</v>
       </c>
       <c r="G62" t="n">
-        <v>3501620</v>
+        <v>3504680</v>
       </c>
       <c r="H62" t="n">
-        <v>161.3399963378906</v>
+        <v>171.7599945068359</v>
       </c>
     </row>
     <row r="63">
@@ -3626,25 +3656,25 @@
         <v>1001</v>
       </c>
       <c r="B63" t="n">
-        <v>5055</v>
+        <v>5357</v>
       </c>
       <c r="C63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D63" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E63" t="n">
-        <v>69.55000305175781</v>
+        <v>80.59999847412109</v>
       </c>
       <c r="F63" t="n">
-        <v>501620</v>
+        <v>506680</v>
       </c>
       <c r="G63" t="n">
-        <v>3501620</v>
+        <v>3504680</v>
       </c>
       <c r="H63" t="n">
-        <v>161.3399963378906</v>
+        <v>171.7599945068359</v>
       </c>
     </row>
     <row r="64">
@@ -3652,25 +3682,25 @@
         <v>1001</v>
       </c>
       <c r="B64" t="n">
-        <v>5056</v>
+        <v>5059</v>
       </c>
       <c r="C64" t="n">
         <v>1</v>
       </c>
       <c r="D64" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E64" t="n">
-        <v>69.73999786376953</v>
+        <v>81.30999755859375</v>
       </c>
       <c r="F64" t="n">
-        <v>501650</v>
+        <v>501740</v>
       </c>
       <c r="G64" t="n">
-        <v>3501650</v>
+        <v>3501740</v>
       </c>
       <c r="H64" t="n">
-        <v>161.5500030517578</v>
+        <v>162.1799926757812</v>
       </c>
     </row>
     <row r="65">
@@ -3678,25 +3708,25 @@
         <v>1001</v>
       </c>
       <c r="B65" t="n">
-        <v>5356</v>
+        <v>5060</v>
       </c>
       <c r="C65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D65" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E65" t="n">
-        <v>68.61000061035156</v>
+        <v>81.05000305175781</v>
       </c>
       <c r="F65" t="n">
-        <v>506650</v>
+        <v>501770</v>
       </c>
       <c r="G65" t="n">
-        <v>3504650</v>
+        <v>3501770</v>
       </c>
       <c r="H65" t="n">
-        <v>171.5500030517578</v>
+        <v>162.3899993896484</v>
       </c>
     </row>
     <row r="66">
@@ -3704,25 +3734,25 @@
         <v>1001</v>
       </c>
       <c r="B66" t="n">
-        <v>5057</v>
+        <v>5060</v>
       </c>
       <c r="C66" t="n">
         <v>1</v>
       </c>
       <c r="D66" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E66" t="n">
-        <v>69.87000274658203</v>
+        <v>80.54000091552734</v>
       </c>
       <c r="F66" t="n">
-        <v>501680</v>
+        <v>501770</v>
       </c>
       <c r="G66" t="n">
-        <v>3501680</v>
+        <v>3501770</v>
       </c>
       <c r="H66" t="n">
-        <v>161.7599945068359</v>
+        <v>162.3899993896484</v>
       </c>
     </row>
     <row r="67">
@@ -3730,25 +3760,25 @@
         <v>1001</v>
       </c>
       <c r="B67" t="n">
-        <v>5059</v>
+        <v>5001</v>
       </c>
       <c r="C67" t="n">
         <v>1</v>
       </c>
       <c r="D67" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E67" t="n">
-        <v>68.94000244140625</v>
+        <v>68.77999877929688</v>
       </c>
       <c r="F67" t="n">
-        <v>501740</v>
+        <v>500000</v>
       </c>
       <c r="G67" t="n">
-        <v>3501740</v>
+        <v>3500000</v>
       </c>
       <c r="H67" t="n">
-        <v>162.1799926757812</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68">
@@ -3756,25 +3786,25 @@
         <v>1001</v>
       </c>
       <c r="B68" t="n">
-        <v>5360</v>
+        <v>5001</v>
       </c>
       <c r="C68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D68" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E68" t="n">
-        <v>68.48999786376953</v>
+        <v>68.79000091552734</v>
       </c>
       <c r="F68" t="n">
-        <v>506770</v>
+        <v>500000</v>
       </c>
       <c r="G68" t="n">
-        <v>3504770</v>
+        <v>3500000</v>
       </c>
       <c r="H68" t="n">
-        <v>172.3899993896484</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69">
@@ -3782,25 +3812,25 @@
         <v>1001</v>
       </c>
       <c r="B69" t="n">
-        <v>5001</v>
+        <v>5301</v>
       </c>
       <c r="C69" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D69" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E69" t="n">
-        <v>68.77999877929688</v>
+        <v>68.26999664306641</v>
       </c>
       <c r="F69" t="n">
-        <v>500000</v>
+        <v>505000</v>
       </c>
       <c r="G69" t="n">
-        <v>3500000</v>
+        <v>3503000</v>
       </c>
       <c r="H69" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="70">
@@ -3808,7 +3838,7 @@
         <v>1001</v>
       </c>
       <c r="B70" t="n">
-        <v>5001</v>
+        <v>5002</v>
       </c>
       <c r="C70" t="n">
         <v>1</v>
@@ -3817,16 +3847,16 @@
         <v>4</v>
       </c>
       <c r="E70" t="n">
-        <v>68.79000091552734</v>
+        <v>69.37000274658203</v>
       </c>
       <c r="F70" t="n">
-        <v>500000</v>
+        <v>500030</v>
       </c>
       <c r="G70" t="n">
-        <v>3500000</v>
+        <v>3500030</v>
       </c>
       <c r="H70" t="n">
-        <v>150</v>
+        <v>150.2100067138672</v>
       </c>
     </row>
     <row r="71">
@@ -3834,7 +3864,7 @@
         <v>1001</v>
       </c>
       <c r="B71" t="n">
-        <v>5301</v>
+        <v>5302</v>
       </c>
       <c r="C71" t="n">
         <v>2</v>
@@ -3843,16 +3873,16 @@
         <v>6</v>
       </c>
       <c r="E71" t="n">
-        <v>68.26999664306641</v>
+        <v>69.51000213623047</v>
       </c>
       <c r="F71" t="n">
-        <v>505000</v>
+        <v>505030</v>
       </c>
       <c r="G71" t="n">
-        <v>3503000</v>
+        <v>3503030</v>
       </c>
       <c r="H71" t="n">
-        <v>160</v>
+        <v>160.2100067138672</v>
       </c>
     </row>
     <row r="72">
@@ -3860,25 +3890,25 @@
         <v>1001</v>
       </c>
       <c r="B72" t="n">
-        <v>5002</v>
+        <v>5003</v>
       </c>
       <c r="C72" t="n">
         <v>1</v>
       </c>
       <c r="D72" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E72" t="n">
-        <v>69.37000274658203</v>
+        <v>68.05999755859375</v>
       </c>
       <c r="F72" t="n">
-        <v>500030</v>
+        <v>500060</v>
       </c>
       <c r="G72" t="n">
-        <v>3500030</v>
+        <v>3500060</v>
       </c>
       <c r="H72" t="n">
-        <v>150.2100067138672</v>
+        <v>150.4199981689453</v>
       </c>
     </row>
     <row r="73">
@@ -3886,25 +3916,25 @@
         <v>1001</v>
       </c>
       <c r="B73" t="n">
-        <v>5302</v>
+        <v>5004</v>
       </c>
       <c r="C73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D73" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E73" t="n">
-        <v>69.51000213623047</v>
+        <v>69.41000366210938</v>
       </c>
       <c r="F73" t="n">
-        <v>505030</v>
+        <v>500090</v>
       </c>
       <c r="G73" t="n">
-        <v>3503030</v>
+        <v>3500090</v>
       </c>
       <c r="H73" t="n">
-        <v>160.2100067138672</v>
+        <v>150.6300048828125</v>
       </c>
     </row>
     <row r="74">
@@ -3912,25 +3942,25 @@
         <v>1001</v>
       </c>
       <c r="B74" t="n">
-        <v>5003</v>
+        <v>5304</v>
       </c>
       <c r="C74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D74" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E74" t="n">
-        <v>68.05999755859375</v>
+        <v>69.16000366210938</v>
       </c>
       <c r="F74" t="n">
-        <v>500060</v>
+        <v>505090</v>
       </c>
       <c r="G74" t="n">
-        <v>3500060</v>
+        <v>3503090</v>
       </c>
       <c r="H74" t="n">
-        <v>150.4199981689453</v>
+        <v>160.6300048828125</v>
       </c>
     </row>
     <row r="75">
@@ -3938,25 +3968,25 @@
         <v>1001</v>
       </c>
       <c r="B75" t="n">
-        <v>5004</v>
+        <v>5306</v>
       </c>
       <c r="C75" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E75" t="n">
-        <v>69.41000366210938</v>
+        <v>69.58000183105469</v>
       </c>
       <c r="F75" t="n">
-        <v>500090</v>
+        <v>505150</v>
       </c>
       <c r="G75" t="n">
-        <v>3500090</v>
+        <v>3503150</v>
       </c>
       <c r="H75" t="n">
-        <v>150.6300048828125</v>
+        <v>161.0500030517578</v>
       </c>
     </row>
     <row r="76">
@@ -3964,25 +3994,25 @@
         <v>1001</v>
       </c>
       <c r="B76" t="n">
-        <v>5304</v>
+        <v>5307</v>
       </c>
       <c r="C76" t="n">
         <v>2</v>
       </c>
       <c r="D76" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E76" t="n">
-        <v>69.16000366210938</v>
+        <v>69.95999908447266</v>
       </c>
       <c r="F76" t="n">
-        <v>505090</v>
+        <v>505180</v>
       </c>
       <c r="G76" t="n">
-        <v>3503090</v>
+        <v>3503180</v>
       </c>
       <c r="H76" t="n">
-        <v>160.6300048828125</v>
+        <v>161.2599945068359</v>
       </c>
     </row>
     <row r="77">
@@ -3990,25 +4020,25 @@
         <v>1001</v>
       </c>
       <c r="B77" t="n">
-        <v>5306</v>
+        <v>5008</v>
       </c>
       <c r="C77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D77" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E77" t="n">
-        <v>69.58000183105469</v>
+        <v>69.22000122070312</v>
       </c>
       <c r="F77" t="n">
-        <v>505150</v>
+        <v>500210</v>
       </c>
       <c r="G77" t="n">
-        <v>3503150</v>
+        <v>3500210</v>
       </c>
       <c r="H77" t="n">
-        <v>161.0500030517578</v>
+        <v>151.4700012207031</v>
       </c>
     </row>
     <row r="78">
@@ -4016,25 +4046,25 @@
         <v>1001</v>
       </c>
       <c r="B78" t="n">
-        <v>5307</v>
+        <v>5308</v>
       </c>
       <c r="C78" t="n">
         <v>2</v>
       </c>
       <c r="D78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E78" t="n">
-        <v>69.95999908447266</v>
+        <v>69.66999816894531</v>
       </c>
       <c r="F78" t="n">
-        <v>505180</v>
+        <v>505210</v>
       </c>
       <c r="G78" t="n">
-        <v>3503180</v>
+        <v>3503210</v>
       </c>
       <c r="H78" t="n">
-        <v>161.2599945068359</v>
+        <v>161.4700012207031</v>
       </c>
     </row>
     <row r="79">
@@ -4042,25 +4072,25 @@
         <v>1001</v>
       </c>
       <c r="B79" t="n">
-        <v>5008</v>
+        <v>5009</v>
       </c>
       <c r="C79" t="n">
         <v>1</v>
       </c>
       <c r="D79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E79" t="n">
-        <v>69.22000122070312</v>
+        <v>69.04000091552734</v>
       </c>
       <c r="F79" t="n">
-        <v>500210</v>
+        <v>500240</v>
       </c>
       <c r="G79" t="n">
-        <v>3500210</v>
+        <v>3500240</v>
       </c>
       <c r="H79" t="n">
-        <v>151.4700012207031</v>
+        <v>151.6799926757812</v>
       </c>
     </row>
     <row r="80">
@@ -4068,25 +4098,25 @@
         <v>1001</v>
       </c>
       <c r="B80" t="n">
-        <v>5308</v>
+        <v>5309</v>
       </c>
       <c r="C80" t="n">
         <v>2</v>
       </c>
       <c r="D80" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E80" t="n">
-        <v>69.66999816894531</v>
+        <v>68.05000305175781</v>
       </c>
       <c r="F80" t="n">
-        <v>505210</v>
+        <v>505240</v>
       </c>
       <c r="G80" t="n">
-        <v>3503210</v>
+        <v>3503240</v>
       </c>
       <c r="H80" t="n">
-        <v>161.4700012207031</v>
+        <v>161.6799926757812</v>
       </c>
     </row>
     <row r="81">
@@ -4094,25 +4124,25 @@
         <v>1001</v>
       </c>
       <c r="B81" t="n">
-        <v>5009</v>
+        <v>5309</v>
       </c>
       <c r="C81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D81" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E81" t="n">
-        <v>69.04000091552734</v>
+        <v>68.01999664306641</v>
       </c>
       <c r="F81" t="n">
-        <v>500240</v>
+        <v>505240</v>
       </c>
       <c r="G81" t="n">
-        <v>3500240</v>
+        <v>3503240</v>
       </c>
       <c r="H81" t="n">
-        <v>151.6799926757812</v>
+        <v>161.6799926757812</v>
       </c>
     </row>
     <row r="82">
@@ -4120,25 +4150,25 @@
         <v>1001</v>
       </c>
       <c r="B82" t="n">
-        <v>5309</v>
+        <v>5010</v>
       </c>
       <c r="C82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D82" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E82" t="n">
-        <v>68.05000305175781</v>
+        <v>69.98999786376953</v>
       </c>
       <c r="F82" t="n">
-        <v>505240</v>
+        <v>500270</v>
       </c>
       <c r="G82" t="n">
-        <v>3503240</v>
+        <v>3500270</v>
       </c>
       <c r="H82" t="n">
-        <v>161.6799926757812</v>
+        <v>151.8899993896484</v>
       </c>
     </row>
     <row r="83">
@@ -4146,25 +4176,25 @@
         <v>1001</v>
       </c>
       <c r="B83" t="n">
-        <v>5309</v>
+        <v>5310</v>
       </c>
       <c r="C83" t="n">
         <v>2</v>
       </c>
       <c r="D83" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E83" t="n">
-        <v>68.01999664306641</v>
+        <v>69.94000244140625</v>
       </c>
       <c r="F83" t="n">
-        <v>505240</v>
+        <v>505270</v>
       </c>
       <c r="G83" t="n">
-        <v>3503240</v>
+        <v>3503270</v>
       </c>
       <c r="H83" t="n">
-        <v>161.6799926757812</v>
+        <v>161.8899993896484</v>
       </c>
     </row>
     <row r="84">
@@ -4172,25 +4202,25 @@
         <v>1001</v>
       </c>
       <c r="B84" t="n">
-        <v>5010</v>
+        <v>5311</v>
       </c>
       <c r="C84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D84" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E84" t="n">
-        <v>69.98999786376953</v>
+        <v>68.95999908447266</v>
       </c>
       <c r="F84" t="n">
-        <v>500270</v>
+        <v>505300</v>
       </c>
       <c r="G84" t="n">
-        <v>3500270</v>
+        <v>3503300</v>
       </c>
       <c r="H84" t="n">
-        <v>151.8899993896484</v>
+        <v>162.1000061035156</v>
       </c>
     </row>
     <row r="85">
@@ -4198,25 +4228,25 @@
         <v>1001</v>
       </c>
       <c r="B85" t="n">
-        <v>5310</v>
+        <v>5012</v>
       </c>
       <c r="C85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D85" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E85" t="n">
-        <v>69.94000244140625</v>
+        <v>68.37000274658203</v>
       </c>
       <c r="F85" t="n">
-        <v>505270</v>
+        <v>500330</v>
       </c>
       <c r="G85" t="n">
-        <v>3503270</v>
+        <v>3500330</v>
       </c>
       <c r="H85" t="n">
-        <v>161.8899993896484</v>
+        <v>152.3099975585938</v>
       </c>
     </row>
     <row r="86">
@@ -4224,7 +4254,7 @@
         <v>1001</v>
       </c>
       <c r="B86" t="n">
-        <v>5311</v>
+        <v>5312</v>
       </c>
       <c r="C86" t="n">
         <v>2</v>
@@ -4233,16 +4263,16 @@
         <v>6</v>
       </c>
       <c r="E86" t="n">
-        <v>68.95999908447266</v>
+        <v>68.09999847412109</v>
       </c>
       <c r="F86" t="n">
-        <v>505300</v>
+        <v>505330</v>
       </c>
       <c r="G86" t="n">
-        <v>3503300</v>
+        <v>3503330</v>
       </c>
       <c r="H86" t="n">
-        <v>162.1000061035156</v>
+        <v>162.3099975585938</v>
       </c>
     </row>
     <row r="87">
@@ -4250,25 +4280,25 @@
         <v>1001</v>
       </c>
       <c r="B87" t="n">
-        <v>5012</v>
+        <v>5015</v>
       </c>
       <c r="C87" t="n">
         <v>1</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E87" t="n">
-        <v>68.37000274658203</v>
+        <v>68.45999908447266</v>
       </c>
       <c r="F87" t="n">
-        <v>500330</v>
+        <v>500420</v>
       </c>
       <c r="G87" t="n">
-        <v>3500330</v>
+        <v>3500420</v>
       </c>
       <c r="H87" t="n">
-        <v>152.3099975585938</v>
+        <v>152.9400024414062</v>
       </c>
     </row>
     <row r="88">
@@ -4276,25 +4306,25 @@
         <v>1001</v>
       </c>
       <c r="B88" t="n">
-        <v>5312</v>
+        <v>5016</v>
       </c>
       <c r="C88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D88" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E88" t="n">
-        <v>68.09999847412109</v>
+        <v>68.68000030517578</v>
       </c>
       <c r="F88" t="n">
-        <v>505330</v>
+        <v>500450</v>
       </c>
       <c r="G88" t="n">
-        <v>3503330</v>
+        <v>3500450</v>
       </c>
       <c r="H88" t="n">
-        <v>162.3099975585938</v>
+        <v>153.1499938964844</v>
       </c>
     </row>
     <row r="89">
@@ -4302,25 +4332,25 @@
         <v>1001</v>
       </c>
       <c r="B89" t="n">
-        <v>5015</v>
+        <v>5018</v>
       </c>
       <c r="C89" t="n">
         <v>1</v>
       </c>
       <c r="D89" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E89" t="n">
-        <v>68.45999908447266</v>
+        <v>68.01999664306641</v>
       </c>
       <c r="F89" t="n">
-        <v>500420</v>
+        <v>500510</v>
       </c>
       <c r="G89" t="n">
-        <v>3500420</v>
+        <v>3500510</v>
       </c>
       <c r="H89" t="n">
-        <v>152.9400024414062</v>
+        <v>153.5700073242188</v>
       </c>
     </row>
     <row r="90">
@@ -4328,25 +4358,25 @@
         <v>1001</v>
       </c>
       <c r="B90" t="n">
-        <v>5016</v>
+        <v>5319</v>
       </c>
       <c r="C90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D90" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E90" t="n">
-        <v>68.68000030517578</v>
+        <v>69.73000335693359</v>
       </c>
       <c r="F90" t="n">
-        <v>500450</v>
+        <v>505540</v>
       </c>
       <c r="G90" t="n">
-        <v>3500450</v>
+        <v>3503540</v>
       </c>
       <c r="H90" t="n">
-        <v>153.1499938964844</v>
+        <v>163.7799987792969</v>
       </c>
     </row>
     <row r="91">
@@ -4354,7 +4384,7 @@
         <v>1001</v>
       </c>
       <c r="B91" t="n">
-        <v>5018</v>
+        <v>5020</v>
       </c>
       <c r="C91" t="n">
         <v>1</v>
@@ -4363,16 +4393,16 @@
         <v>1</v>
       </c>
       <c r="E91" t="n">
-        <v>68.01999664306641</v>
+        <v>69.29000091552734</v>
       </c>
       <c r="F91" t="n">
-        <v>500510</v>
+        <v>500570</v>
       </c>
       <c r="G91" t="n">
-        <v>3500510</v>
+        <v>3500570</v>
       </c>
       <c r="H91" t="n">
-        <v>153.5700073242188</v>
+        <v>153.9900054931641</v>
       </c>
     </row>
     <row r="92">
@@ -4380,25 +4410,25 @@
         <v>1001</v>
       </c>
       <c r="B92" t="n">
-        <v>5319</v>
+        <v>5320</v>
       </c>
       <c r="C92" t="n">
         <v>2</v>
       </c>
       <c r="D92" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E92" t="n">
-        <v>69.73000335693359</v>
+        <v>68.13999938964844</v>
       </c>
       <c r="F92" t="n">
-        <v>505540</v>
+        <v>505570</v>
       </c>
       <c r="G92" t="n">
-        <v>3503540</v>
+        <v>3503570</v>
       </c>
       <c r="H92" t="n">
-        <v>163.7799987792969</v>
+        <v>163.9900054931641</v>
       </c>
     </row>
     <row r="93">
@@ -4406,25 +4436,25 @@
         <v>1001</v>
       </c>
       <c r="B93" t="n">
-        <v>5020</v>
+        <v>5321</v>
       </c>
       <c r="C93" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D93" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E93" t="n">
-        <v>69.29000091552734</v>
+        <v>68.34999847412109</v>
       </c>
       <c r="F93" t="n">
-        <v>500570</v>
+        <v>505600</v>
       </c>
       <c r="G93" t="n">
-        <v>3500570</v>
+        <v>3503600</v>
       </c>
       <c r="H93" t="n">
-        <v>153.9900054931641</v>
+        <v>164.1999969482422</v>
       </c>
     </row>
     <row r="94">
@@ -4432,25 +4462,25 @@
         <v>1001</v>
       </c>
       <c r="B94" t="n">
-        <v>5320</v>
+        <v>5022</v>
       </c>
       <c r="C94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D94" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E94" t="n">
-        <v>68.13999938964844</v>
+        <v>68.80000305175781</v>
       </c>
       <c r="F94" t="n">
-        <v>505570</v>
+        <v>500630</v>
       </c>
       <c r="G94" t="n">
-        <v>3503570</v>
+        <v>3500630</v>
       </c>
       <c r="H94" t="n">
-        <v>163.9900054931641</v>
+        <v>154.4100036621094</v>
       </c>
     </row>
     <row r="95">
@@ -4458,25 +4488,25 @@
         <v>1001</v>
       </c>
       <c r="B95" t="n">
-        <v>5321</v>
+        <v>5023</v>
       </c>
       <c r="C95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D95" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E95" t="n">
-        <v>68.34999847412109</v>
+        <v>69.62999725341797</v>
       </c>
       <c r="F95" t="n">
-        <v>505600</v>
+        <v>500660</v>
       </c>
       <c r="G95" t="n">
-        <v>3503600</v>
+        <v>3500660</v>
       </c>
       <c r="H95" t="n">
-        <v>164.1999969482422</v>
+        <v>154.6199951171875</v>
       </c>
     </row>
     <row r="96">
@@ -4484,25 +4514,25 @@
         <v>1001</v>
       </c>
       <c r="B96" t="n">
-        <v>5022</v>
+        <v>5023</v>
       </c>
       <c r="C96" t="n">
         <v>1</v>
       </c>
       <c r="D96" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E96" t="n">
-        <v>68.80000305175781</v>
+        <v>68.80999755859375</v>
       </c>
       <c r="F96" t="n">
-        <v>500630</v>
+        <v>500660</v>
       </c>
       <c r="G96" t="n">
-        <v>3500630</v>
+        <v>3500660</v>
       </c>
       <c r="H96" t="n">
-        <v>154.4100036621094</v>
+        <v>154.6199951171875</v>
       </c>
     </row>
     <row r="97">
@@ -4510,25 +4540,25 @@
         <v>1001</v>
       </c>
       <c r="B97" t="n">
-        <v>5023</v>
+        <v>5025</v>
       </c>
       <c r="C97" t="n">
         <v>1</v>
       </c>
       <c r="D97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E97" t="n">
-        <v>69.62999725341797</v>
+        <v>69.83999633789062</v>
       </c>
       <c r="F97" t="n">
-        <v>500660</v>
+        <v>500720</v>
       </c>
       <c r="G97" t="n">
-        <v>3500660</v>
+        <v>3500720</v>
       </c>
       <c r="H97" t="n">
-        <v>154.6199951171875</v>
+        <v>155.0399932861328</v>
       </c>
     </row>
     <row r="98">
@@ -4536,7 +4566,7 @@
         <v>1001</v>
       </c>
       <c r="B98" t="n">
-        <v>5023</v>
+        <v>5025</v>
       </c>
       <c r="C98" t="n">
         <v>1</v>
@@ -4545,16 +4575,16 @@
         <v>4</v>
       </c>
       <c r="E98" t="n">
-        <v>68.80999755859375</v>
+        <v>69.27999877929688</v>
       </c>
       <c r="F98" t="n">
-        <v>500660</v>
+        <v>500720</v>
       </c>
       <c r="G98" t="n">
-        <v>3500660</v>
+        <v>3500720</v>
       </c>
       <c r="H98" t="n">
-        <v>154.6199951171875</v>
+        <v>155.0399932861328</v>
       </c>
     </row>
     <row r="99">
@@ -4562,25 +4592,25 @@
         <v>1001</v>
       </c>
       <c r="B99" t="n">
-        <v>5025</v>
+        <v>5325</v>
       </c>
       <c r="C99" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D99" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E99" t="n">
-        <v>69.83999633789062</v>
+        <v>68.15000152587891</v>
       </c>
       <c r="F99" t="n">
-        <v>500720</v>
+        <v>505720</v>
       </c>
       <c r="G99" t="n">
-        <v>3500720</v>
+        <v>3503720</v>
       </c>
       <c r="H99" t="n">
-        <v>155.0399932861328</v>
+        <v>165.0399932861328</v>
       </c>
     </row>
     <row r="100">
@@ -4588,7 +4618,7 @@
         <v>1001</v>
       </c>
       <c r="B100" t="n">
-        <v>5025</v>
+        <v>5026</v>
       </c>
       <c r="C100" t="n">
         <v>1</v>
@@ -4597,16 +4627,16 @@
         <v>4</v>
       </c>
       <c r="E100" t="n">
-        <v>69.27999877929688</v>
+        <v>68.86000061035156</v>
       </c>
       <c r="F100" t="n">
-        <v>500720</v>
+        <v>500750</v>
       </c>
       <c r="G100" t="n">
-        <v>3500720</v>
+        <v>3500750</v>
       </c>
       <c r="H100" t="n">
-        <v>155.0399932861328</v>
+        <v>155.25</v>
       </c>
     </row>
     <row r="101">
@@ -4614,25 +4644,25 @@
         <v>1001</v>
       </c>
       <c r="B101" t="n">
-        <v>5325</v>
+        <v>5028</v>
       </c>
       <c r="C101" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D101" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E101" t="n">
-        <v>68.15000152587891</v>
+        <v>69.26000213623047</v>
       </c>
       <c r="F101" t="n">
-        <v>505720</v>
+        <v>500810</v>
       </c>
       <c r="G101" t="n">
-        <v>3503720</v>
+        <v>3500810</v>
       </c>
       <c r="H101" t="n">
-        <v>165.0399932861328</v>
+        <v>155.6699981689453</v>
       </c>
     </row>
     <row r="102">
@@ -4640,25 +4670,25 @@
         <v>1001</v>
       </c>
       <c r="B102" t="n">
-        <v>5026</v>
+        <v>5329</v>
       </c>
       <c r="C102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D102" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E102" t="n">
-        <v>68.86000061035156</v>
+        <v>69.26000213623047</v>
       </c>
       <c r="F102" t="n">
-        <v>500750</v>
+        <v>505840</v>
       </c>
       <c r="G102" t="n">
-        <v>3500750</v>
+        <v>3503840</v>
       </c>
       <c r="H102" t="n">
-        <v>155.25</v>
+        <v>165.8800048828125</v>
       </c>
     </row>
     <row r="103">
@@ -4666,25 +4696,25 @@
         <v>1001</v>
       </c>
       <c r="B103" t="n">
-        <v>5028</v>
+        <v>5030</v>
       </c>
       <c r="C103" t="n">
         <v>1</v>
       </c>
       <c r="D103" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E103" t="n">
-        <v>69.26000213623047</v>
+        <v>68.84999847412109</v>
       </c>
       <c r="F103" t="n">
-        <v>500810</v>
+        <v>500870</v>
       </c>
       <c r="G103" t="n">
-        <v>3500810</v>
+        <v>3500870</v>
       </c>
       <c r="H103" t="n">
-        <v>155.6699981689453</v>
+        <v>156.0899963378906</v>
       </c>
     </row>
     <row r="104">
@@ -4692,25 +4722,25 @@
         <v>1001</v>
       </c>
       <c r="B104" t="n">
-        <v>5329</v>
+        <v>5031</v>
       </c>
       <c r="C104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D104" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E104" t="n">
-        <v>69.26000213623047</v>
+        <v>69.54000091552734</v>
       </c>
       <c r="F104" t="n">
-        <v>505840</v>
+        <v>500900</v>
       </c>
       <c r="G104" t="n">
-        <v>3503840</v>
+        <v>3500900</v>
       </c>
       <c r="H104" t="n">
-        <v>165.8800048828125</v>
+        <v>156.3000030517578</v>
       </c>
     </row>
     <row r="105">
@@ -4718,25 +4748,25 @@
         <v>1001</v>
       </c>
       <c r="B105" t="n">
-        <v>5030</v>
+        <v>5031</v>
       </c>
       <c r="C105" t="n">
         <v>1</v>
       </c>
       <c r="D105" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E105" t="n">
-        <v>68.84999847412109</v>
+        <v>69.54000091552734</v>
       </c>
       <c r="F105" t="n">
-        <v>500870</v>
+        <v>500900</v>
       </c>
       <c r="G105" t="n">
-        <v>3500870</v>
+        <v>3500900</v>
       </c>
       <c r="H105" t="n">
-        <v>156.0899963378906</v>
+        <v>156.3000030517578</v>
       </c>
     </row>
     <row r="106">
@@ -4744,25 +4774,25 @@
         <v>1001</v>
       </c>
       <c r="B106" t="n">
-        <v>5031</v>
+        <v>5332</v>
       </c>
       <c r="C106" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D106" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E106" t="n">
-        <v>69.54000091552734</v>
+        <v>69.23999786376953</v>
       </c>
       <c r="F106" t="n">
-        <v>500900</v>
+        <v>505930</v>
       </c>
       <c r="G106" t="n">
-        <v>3500900</v>
+        <v>3503930</v>
       </c>
       <c r="H106" t="n">
-        <v>156.3000030517578</v>
+        <v>166.5099945068359</v>
       </c>
     </row>
     <row r="107">
@@ -4770,25 +4800,25 @@
         <v>1001</v>
       </c>
       <c r="B107" t="n">
-        <v>5031</v>
+        <v>5033</v>
       </c>
       <c r="C107" t="n">
         <v>1</v>
       </c>
       <c r="D107" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E107" t="n">
-        <v>69.54000091552734</v>
+        <v>68.84999847412109</v>
       </c>
       <c r="F107" t="n">
-        <v>500900</v>
+        <v>500960</v>
       </c>
       <c r="G107" t="n">
-        <v>3500900</v>
+        <v>3500960</v>
       </c>
       <c r="H107" t="n">
-        <v>156.3000030517578</v>
+        <v>156.7200012207031</v>
       </c>
     </row>
     <row r="108">
@@ -4796,25 +4826,25 @@
         <v>1001</v>
       </c>
       <c r="B108" t="n">
-        <v>5332</v>
+        <v>5334</v>
       </c>
       <c r="C108" t="n">
         <v>2</v>
       </c>
       <c r="D108" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E108" t="n">
-        <v>69.23999786376953</v>
+        <v>69.87000274658203</v>
       </c>
       <c r="F108" t="n">
-        <v>505930</v>
+        <v>505990</v>
       </c>
       <c r="G108" t="n">
-        <v>3503930</v>
+        <v>3503990</v>
       </c>
       <c r="H108" t="n">
-        <v>166.5099945068359</v>
+        <v>166.9299926757812</v>
       </c>
     </row>
     <row r="109">
@@ -4822,25 +4852,25 @@
         <v>1001</v>
       </c>
       <c r="B109" t="n">
-        <v>5033</v>
+        <v>5335</v>
       </c>
       <c r="C109" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D109" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E109" t="n">
-        <v>68.84999847412109</v>
+        <v>68.45999908447266</v>
       </c>
       <c r="F109" t="n">
-        <v>500960</v>
+        <v>506020</v>
       </c>
       <c r="G109" t="n">
-        <v>3500960</v>
+        <v>3504020</v>
       </c>
       <c r="H109" t="n">
-        <v>156.7200012207031</v>
+        <v>167.1399993896484</v>
       </c>
     </row>
     <row r="110">
@@ -4848,25 +4878,25 @@
         <v>1001</v>
       </c>
       <c r="B110" t="n">
-        <v>5334</v>
+        <v>5335</v>
       </c>
       <c r="C110" t="n">
         <v>2</v>
       </c>
       <c r="D110" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E110" t="n">
-        <v>69.87000274658203</v>
+        <v>68.75</v>
       </c>
       <c r="F110" t="n">
-        <v>505990</v>
+        <v>506020</v>
       </c>
       <c r="G110" t="n">
-        <v>3503990</v>
+        <v>3504020</v>
       </c>
       <c r="H110" t="n">
-        <v>166.9299926757812</v>
+        <v>167.1399993896484</v>
       </c>
     </row>
     <row r="111">
@@ -4874,25 +4904,25 @@
         <v>1001</v>
       </c>
       <c r="B111" t="n">
-        <v>5335</v>
+        <v>5037</v>
       </c>
       <c r="C111" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D111" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E111" t="n">
-        <v>68.45999908447266</v>
+        <v>69.05999755859375</v>
       </c>
       <c r="F111" t="n">
-        <v>506020</v>
+        <v>501080</v>
       </c>
       <c r="G111" t="n">
-        <v>3504020</v>
+        <v>3501080</v>
       </c>
       <c r="H111" t="n">
-        <v>167.1399993896484</v>
+        <v>157.5599975585938</v>
       </c>
     </row>
     <row r="112">
@@ -4900,25 +4930,25 @@
         <v>1001</v>
       </c>
       <c r="B112" t="n">
-        <v>5335</v>
+        <v>5039</v>
       </c>
       <c r="C112" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D112" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E112" t="n">
-        <v>68.75</v>
+        <v>69.02999877929688</v>
       </c>
       <c r="F112" t="n">
-        <v>506020</v>
+        <v>501140</v>
       </c>
       <c r="G112" t="n">
-        <v>3504020</v>
+        <v>3501140</v>
       </c>
       <c r="H112" t="n">
-        <v>167.1399993896484</v>
+        <v>157.9799957275391</v>
       </c>
     </row>
     <row r="113">
@@ -4926,25 +4956,25 @@
         <v>1001</v>
       </c>
       <c r="B113" t="n">
-        <v>5037</v>
+        <v>5040</v>
       </c>
       <c r="C113" t="n">
         <v>1</v>
       </c>
       <c r="D113" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E113" t="n">
-        <v>69.05999755859375</v>
+        <v>68.55000305175781</v>
       </c>
       <c r="F113" t="n">
-        <v>501080</v>
+        <v>501170</v>
       </c>
       <c r="G113" t="n">
-        <v>3501080</v>
+        <v>3501170</v>
       </c>
       <c r="H113" t="n">
-        <v>157.5599975585938</v>
+        <v>158.1900024414062</v>
       </c>
     </row>
     <row r="114">
@@ -4952,25 +4982,25 @@
         <v>1001</v>
       </c>
       <c r="B114" t="n">
-        <v>5039</v>
+        <v>5043</v>
       </c>
       <c r="C114" t="n">
         <v>1</v>
       </c>
       <c r="D114" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E114" t="n">
-        <v>69.02999877929688</v>
+        <v>69.62000274658203</v>
       </c>
       <c r="F114" t="n">
-        <v>501140</v>
+        <v>501260</v>
       </c>
       <c r="G114" t="n">
-        <v>3501140</v>
+        <v>3501260</v>
       </c>
       <c r="H114" t="n">
-        <v>157.9799957275391</v>
+        <v>158.8200073242188</v>
       </c>
     </row>
     <row r="115">
@@ -4978,7 +5008,7 @@
         <v>1001</v>
       </c>
       <c r="B115" t="n">
-        <v>5040</v>
+        <v>5043</v>
       </c>
       <c r="C115" t="n">
         <v>1</v>
@@ -4987,16 +5017,16 @@
         <v>2</v>
       </c>
       <c r="E115" t="n">
-        <v>68.55000305175781</v>
+        <v>68.72000122070312</v>
       </c>
       <c r="F115" t="n">
-        <v>501170</v>
+        <v>501260</v>
       </c>
       <c r="G115" t="n">
-        <v>3501170</v>
+        <v>3501260</v>
       </c>
       <c r="H115" t="n">
-        <v>158.1900024414062</v>
+        <v>158.8200073242188</v>
       </c>
     </row>
     <row r="116">
@@ -5004,25 +5034,25 @@
         <v>1001</v>
       </c>
       <c r="B116" t="n">
-        <v>5043</v>
+        <v>5044</v>
       </c>
       <c r="C116" t="n">
         <v>1</v>
       </c>
       <c r="D116" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E116" t="n">
-        <v>69.62000274658203</v>
+        <v>68.23000335693359</v>
       </c>
       <c r="F116" t="n">
-        <v>501260</v>
+        <v>501290</v>
       </c>
       <c r="G116" t="n">
-        <v>3501260</v>
+        <v>3501290</v>
       </c>
       <c r="H116" t="n">
-        <v>158.8200073242188</v>
+        <v>159.0299987792969</v>
       </c>
     </row>
     <row r="117">
@@ -5030,25 +5060,25 @@
         <v>1001</v>
       </c>
       <c r="B117" t="n">
-        <v>5043</v>
+        <v>5348</v>
       </c>
       <c r="C117" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D117" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E117" t="n">
-        <v>68.72000122070312</v>
+        <v>69</v>
       </c>
       <c r="F117" t="n">
-        <v>501260</v>
+        <v>506410</v>
       </c>
       <c r="G117" t="n">
-        <v>3501260</v>
+        <v>3504410</v>
       </c>
       <c r="H117" t="n">
-        <v>158.8200073242188</v>
+        <v>169.8699951171875</v>
       </c>
     </row>
     <row r="118">
@@ -5056,25 +5086,25 @@
         <v>1001</v>
       </c>
       <c r="B118" t="n">
-        <v>5044</v>
+        <v>5049</v>
       </c>
       <c r="C118" t="n">
         <v>1</v>
       </c>
       <c r="D118" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E118" t="n">
-        <v>68.23000335693359</v>
+        <v>69.30000305175781</v>
       </c>
       <c r="F118" t="n">
-        <v>501290</v>
+        <v>501440</v>
       </c>
       <c r="G118" t="n">
-        <v>3501290</v>
+        <v>3501440</v>
       </c>
       <c r="H118" t="n">
-        <v>159.0299987792969</v>
+        <v>160.0800018310547</v>
       </c>
     </row>
     <row r="119">
@@ -5082,25 +5112,25 @@
         <v>1001</v>
       </c>
       <c r="B119" t="n">
-        <v>5348</v>
+        <v>5049</v>
       </c>
       <c r="C119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D119" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E119" t="n">
-        <v>69</v>
+        <v>68.12999725341797</v>
       </c>
       <c r="F119" t="n">
-        <v>506410</v>
+        <v>501440</v>
       </c>
       <c r="G119" t="n">
-        <v>3504410</v>
+        <v>3501440</v>
       </c>
       <c r="H119" t="n">
-        <v>169.8699951171875</v>
+        <v>160.0800018310547</v>
       </c>
     </row>
     <row r="120">
@@ -5108,25 +5138,25 @@
         <v>1001</v>
       </c>
       <c r="B120" t="n">
-        <v>5049</v>
+        <v>5349</v>
       </c>
       <c r="C120" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D120" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E120" t="n">
-        <v>69.30000305175781</v>
+        <v>68.01999664306641</v>
       </c>
       <c r="F120" t="n">
-        <v>501440</v>
+        <v>506440</v>
       </c>
       <c r="G120" t="n">
-        <v>3501440</v>
+        <v>3504440</v>
       </c>
       <c r="H120" t="n">
-        <v>160.0800018310547</v>
+        <v>170.0800018310547</v>
       </c>
     </row>
     <row r="121">
@@ -5134,25 +5164,25 @@
         <v>1001</v>
       </c>
       <c r="B121" t="n">
-        <v>5049</v>
+        <v>5349</v>
       </c>
       <c r="C121" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D121" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E121" t="n">
-        <v>68.12999725341797</v>
+        <v>68.43000030517578</v>
       </c>
       <c r="F121" t="n">
-        <v>501440</v>
+        <v>506440</v>
       </c>
       <c r="G121" t="n">
-        <v>3501440</v>
+        <v>3504440</v>
       </c>
       <c r="H121" t="n">
-        <v>160.0800018310547</v>
+        <v>170.0800018310547</v>
       </c>
     </row>
     <row r="122">
@@ -5160,25 +5190,25 @@
         <v>1001</v>
       </c>
       <c r="B122" t="n">
-        <v>5349</v>
+        <v>5050</v>
       </c>
       <c r="C122" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D122" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E122" t="n">
-        <v>68.01999664306641</v>
+        <v>69.77999877929688</v>
       </c>
       <c r="F122" t="n">
-        <v>506440</v>
+        <v>501470</v>
       </c>
       <c r="G122" t="n">
-        <v>3504440</v>
+        <v>3501470</v>
       </c>
       <c r="H122" t="n">
-        <v>170.0800018310547</v>
+        <v>160.2899932861328</v>
       </c>
     </row>
     <row r="123">
@@ -5186,25 +5216,25 @@
         <v>1001</v>
       </c>
       <c r="B123" t="n">
-        <v>5349</v>
+        <v>5050</v>
       </c>
       <c r="C123" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D123" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E123" t="n">
-        <v>68.43000030517578</v>
+        <v>68.12000274658203</v>
       </c>
       <c r="F123" t="n">
-        <v>506440</v>
+        <v>501470</v>
       </c>
       <c r="G123" t="n">
-        <v>3504440</v>
+        <v>3501470</v>
       </c>
       <c r="H123" t="n">
-        <v>170.0800018310547</v>
+        <v>160.2899932861328</v>
       </c>
     </row>
     <row r="124">
@@ -5212,25 +5242,25 @@
         <v>1001</v>
       </c>
       <c r="B124" t="n">
-        <v>5050</v>
+        <v>5051</v>
       </c>
       <c r="C124" t="n">
         <v>1</v>
       </c>
       <c r="D124" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E124" t="n">
-        <v>69.77999877929688</v>
+        <v>68.69000244140625</v>
       </c>
       <c r="F124" t="n">
-        <v>501470</v>
+        <v>501500</v>
       </c>
       <c r="G124" t="n">
-        <v>3501470</v>
+        <v>3501500</v>
       </c>
       <c r="H124" t="n">
-        <v>160.2899932861328</v>
+        <v>160.5</v>
       </c>
     </row>
     <row r="125">
@@ -5238,25 +5268,25 @@
         <v>1001</v>
       </c>
       <c r="B125" t="n">
-        <v>5050</v>
+        <v>5051</v>
       </c>
       <c r="C125" t="n">
         <v>1</v>
       </c>
       <c r="D125" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E125" t="n">
-        <v>68.12000274658203</v>
+        <v>68.69000244140625</v>
       </c>
       <c r="F125" t="n">
-        <v>501470</v>
+        <v>501500</v>
       </c>
       <c r="G125" t="n">
-        <v>3501470</v>
+        <v>3501500</v>
       </c>
       <c r="H125" t="n">
-        <v>160.2899932861328</v>
+        <v>160.5</v>
       </c>
     </row>
     <row r="126">
@@ -5270,10 +5300,10 @@
         <v>1</v>
       </c>
       <c r="D126" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E126" t="n">
-        <v>68.69000244140625</v>
+        <v>69.27999877929688</v>
       </c>
       <c r="F126" t="n">
         <v>501500</v>
@@ -5290,25 +5320,25 @@
         <v>1001</v>
       </c>
       <c r="B127" t="n">
-        <v>5051</v>
+        <v>5354</v>
       </c>
       <c r="C127" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D127" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E127" t="n">
-        <v>68.69000244140625</v>
+        <v>69.77999877929688</v>
       </c>
       <c r="F127" t="n">
-        <v>501500</v>
+        <v>506590</v>
       </c>
       <c r="G127" t="n">
-        <v>3501500</v>
+        <v>3504590</v>
       </c>
       <c r="H127" t="n">
-        <v>160.5</v>
+        <v>171.1300048828125</v>
       </c>
     </row>
     <row r="128">
@@ -5316,25 +5346,25 @@
         <v>1001</v>
       </c>
       <c r="B128" t="n">
-        <v>5051</v>
+        <v>5055</v>
       </c>
       <c r="C128" t="n">
         <v>1</v>
       </c>
       <c r="D128" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E128" t="n">
-        <v>69.27999877929688</v>
+        <v>68.33000183105469</v>
       </c>
       <c r="F128" t="n">
-        <v>501500</v>
+        <v>501620</v>
       </c>
       <c r="G128" t="n">
-        <v>3501500</v>
+        <v>3501620</v>
       </c>
       <c r="H128" t="n">
-        <v>160.5</v>
+        <v>161.3399963378906</v>
       </c>
     </row>
     <row r="129">
@@ -5342,25 +5372,25 @@
         <v>1001</v>
       </c>
       <c r="B129" t="n">
-        <v>5354</v>
+        <v>5055</v>
       </c>
       <c r="C129" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D129" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E129" t="n">
-        <v>69.77999877929688</v>
+        <v>69.55000305175781</v>
       </c>
       <c r="F129" t="n">
-        <v>506590</v>
+        <v>501620</v>
       </c>
       <c r="G129" t="n">
-        <v>3504590</v>
+        <v>3501620</v>
       </c>
       <c r="H129" t="n">
-        <v>171.1300048828125</v>
+        <v>161.3399963378906</v>
       </c>
     </row>
     <row r="130">
@@ -5368,25 +5398,25 @@
         <v>1001</v>
       </c>
       <c r="B130" t="n">
-        <v>5055</v>
+        <v>5056</v>
       </c>
       <c r="C130" t="n">
         <v>1</v>
       </c>
       <c r="D130" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E130" t="n">
-        <v>68.33000183105469</v>
+        <v>69.73999786376953</v>
       </c>
       <c r="F130" t="n">
-        <v>501620</v>
+        <v>501650</v>
       </c>
       <c r="G130" t="n">
-        <v>3501620</v>
+        <v>3501650</v>
       </c>
       <c r="H130" t="n">
-        <v>161.3399963378906</v>
+        <v>161.5500030517578</v>
       </c>
     </row>
     <row r="131">
@@ -5394,25 +5424,25 @@
         <v>1001</v>
       </c>
       <c r="B131" t="n">
-        <v>5055</v>
+        <v>5356</v>
       </c>
       <c r="C131" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D131" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E131" t="n">
-        <v>69.55000305175781</v>
+        <v>68.61000061035156</v>
       </c>
       <c r="F131" t="n">
-        <v>501620</v>
+        <v>506650</v>
       </c>
       <c r="G131" t="n">
-        <v>3501620</v>
+        <v>3504650</v>
       </c>
       <c r="H131" t="n">
-        <v>161.3399963378906</v>
+        <v>171.5500030517578</v>
       </c>
     </row>
     <row r="132">
@@ -5420,25 +5450,25 @@
         <v>1001</v>
       </c>
       <c r="B132" t="n">
-        <v>5056</v>
+        <v>5057</v>
       </c>
       <c r="C132" t="n">
         <v>1</v>
       </c>
       <c r="D132" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E132" t="n">
-        <v>69.73999786376953</v>
+        <v>69.87000274658203</v>
       </c>
       <c r="F132" t="n">
-        <v>501650</v>
+        <v>501680</v>
       </c>
       <c r="G132" t="n">
-        <v>3501650</v>
+        <v>3501680</v>
       </c>
       <c r="H132" t="n">
-        <v>161.5500030517578</v>
+        <v>161.7599945068359</v>
       </c>
     </row>
     <row r="133">
@@ -5446,25 +5476,25 @@
         <v>1001</v>
       </c>
       <c r="B133" t="n">
-        <v>5356</v>
+        <v>5059</v>
       </c>
       <c r="C133" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D133" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E133" t="n">
-        <v>68.61000061035156</v>
+        <v>68.94000244140625</v>
       </c>
       <c r="F133" t="n">
-        <v>506650</v>
+        <v>501740</v>
       </c>
       <c r="G133" t="n">
-        <v>3504650</v>
+        <v>3501740</v>
       </c>
       <c r="H133" t="n">
-        <v>171.5500030517578</v>
+        <v>162.1799926757812</v>
       </c>
     </row>
     <row r="134">
@@ -5472,76 +5502,24 @@
         <v>1001</v>
       </c>
       <c r="B134" t="n">
-        <v>5057</v>
+        <v>5360</v>
       </c>
       <c r="C134" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D134" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E134" t="n">
-        <v>69.87000274658203</v>
+        <v>68.48999786376953</v>
       </c>
       <c r="F134" t="n">
-        <v>501680</v>
+        <v>506770</v>
       </c>
       <c r="G134" t="n">
-        <v>3501680</v>
+        <v>3504770</v>
       </c>
       <c r="H134" t="n">
-        <v>161.7599945068359</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="n">
-        <v>1001</v>
-      </c>
-      <c r="B135" t="n">
-        <v>5059</v>
-      </c>
-      <c r="C135" t="n">
-        <v>1</v>
-      </c>
-      <c r="D135" t="n">
-        <v>1</v>
-      </c>
-      <c r="E135" t="n">
-        <v>68.94000244140625</v>
-      </c>
-      <c r="F135" t="n">
-        <v>501740</v>
-      </c>
-      <c r="G135" t="n">
-        <v>3501740</v>
-      </c>
-      <c r="H135" t="n">
-        <v>162.1799926757812</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="n">
-        <v>1001</v>
-      </c>
-      <c r="B136" t="n">
-        <v>5360</v>
-      </c>
-      <c r="C136" t="n">
-        <v>2</v>
-      </c>
-      <c r="D136" t="n">
-        <v>8</v>
-      </c>
-      <c r="E136" t="n">
-        <v>68.48999786376953</v>
-      </c>
-      <c r="F136" t="n">
-        <v>506770</v>
-      </c>
-      <c r="G136" t="n">
-        <v>3504770</v>
-      </c>
-      <c r="H136" t="n">
         <v>172.3899993896484</v>
       </c>
     </row>

</xml_diff>